<commit_message>
Amelioration Interface+ Ajout bootstrap
</commit_message>
<xml_diff>
--- a/Extraction/etape2bis_conversion.xlsx
+++ b/Extraction/etape2bis_conversion.xlsx
@@ -9905,7 +9905,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:D3200"/>
+  <dimension ref="A1:D4800"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -36027,6 +36027,4806 @@
     <row r="3200" spans="1:4">
       <c r="A3200"/>
     </row>
+    <row r="3201" spans="1:4">
+      <c r="A3201"/>
+    </row>
+    <row r="3202" spans="1:4">
+      <c r="A3202"/>
+    </row>
+    <row r="3203" spans="1:4">
+      <c r="A3203"/>
+    </row>
+    <row r="3204" spans="1:4">
+      <c r="A3204"/>
+    </row>
+    <row r="3205" spans="1:4">
+      <c r="A3205"/>
+    </row>
+    <row r="3206" spans="1:4">
+      <c r="A3206"/>
+    </row>
+    <row r="3207" spans="1:4">
+      <c r="A3207"/>
+    </row>
+    <row r="3208" spans="1:4">
+      <c r="A3208"/>
+    </row>
+    <row r="3209" spans="1:4">
+      <c r="A3209"/>
+    </row>
+    <row r="3210" spans="1:4">
+      <c r="A3210"/>
+    </row>
+    <row r="3211" spans="1:4">
+      <c r="A3211"/>
+    </row>
+    <row r="3212" spans="1:4">
+      <c r="A3212"/>
+    </row>
+    <row r="3213" spans="1:4">
+      <c r="A3213"/>
+    </row>
+    <row r="3214" spans="1:4">
+      <c r="A3214"/>
+    </row>
+    <row r="3215" spans="1:4">
+      <c r="A3215"/>
+    </row>
+    <row r="3216" spans="1:4">
+      <c r="A3216"/>
+    </row>
+    <row r="3217" spans="1:4">
+      <c r="A3217"/>
+    </row>
+    <row r="3218" spans="1:4">
+      <c r="A3218"/>
+    </row>
+    <row r="3219" spans="1:4">
+      <c r="A3219"/>
+    </row>
+    <row r="3220" spans="1:4">
+      <c r="A3220"/>
+    </row>
+    <row r="3221" spans="1:4">
+      <c r="A3221"/>
+    </row>
+    <row r="3222" spans="1:4">
+      <c r="A3222"/>
+    </row>
+    <row r="3223" spans="1:4">
+      <c r="A3223"/>
+    </row>
+    <row r="3224" spans="1:4">
+      <c r="A3224"/>
+    </row>
+    <row r="3225" spans="1:4">
+      <c r="A3225"/>
+    </row>
+    <row r="3226" spans="1:4">
+      <c r="A3226"/>
+    </row>
+    <row r="3227" spans="1:4">
+      <c r="A3227"/>
+    </row>
+    <row r="3228" spans="1:4">
+      <c r="A3228"/>
+    </row>
+    <row r="3229" spans="1:4">
+      <c r="A3229"/>
+    </row>
+    <row r="3230" spans="1:4">
+      <c r="A3230"/>
+    </row>
+    <row r="3231" spans="1:4">
+      <c r="A3231"/>
+    </row>
+    <row r="3232" spans="1:4">
+      <c r="A3232"/>
+    </row>
+    <row r="3233" spans="1:4">
+      <c r="A3233"/>
+    </row>
+    <row r="3234" spans="1:4">
+      <c r="A3234"/>
+    </row>
+    <row r="3235" spans="1:4">
+      <c r="A3235"/>
+    </row>
+    <row r="3236" spans="1:4">
+      <c r="A3236"/>
+    </row>
+    <row r="3237" spans="1:4">
+      <c r="A3237"/>
+    </row>
+    <row r="3238" spans="1:4">
+      <c r="A3238"/>
+    </row>
+    <row r="3239" spans="1:4">
+      <c r="A3239"/>
+    </row>
+    <row r="3240" spans="1:4">
+      <c r="A3240"/>
+    </row>
+    <row r="3241" spans="1:4">
+      <c r="A3241"/>
+    </row>
+    <row r="3242" spans="1:4">
+      <c r="A3242"/>
+    </row>
+    <row r="3243" spans="1:4">
+      <c r="A3243"/>
+    </row>
+    <row r="3244" spans="1:4">
+      <c r="A3244"/>
+    </row>
+    <row r="3245" spans="1:4">
+      <c r="A3245"/>
+    </row>
+    <row r="3246" spans="1:4">
+      <c r="A3246"/>
+    </row>
+    <row r="3247" spans="1:4">
+      <c r="A3247"/>
+    </row>
+    <row r="3248" spans="1:4">
+      <c r="A3248"/>
+    </row>
+    <row r="3249" spans="1:4">
+      <c r="A3249"/>
+    </row>
+    <row r="3250" spans="1:4">
+      <c r="A3250"/>
+    </row>
+    <row r="3251" spans="1:4">
+      <c r="A3251"/>
+    </row>
+    <row r="3252" spans="1:4">
+      <c r="A3252"/>
+    </row>
+    <row r="3253" spans="1:4">
+      <c r="A3253"/>
+    </row>
+    <row r="3254" spans="1:4">
+      <c r="A3254"/>
+    </row>
+    <row r="3255" spans="1:4">
+      <c r="A3255"/>
+    </row>
+    <row r="3256" spans="1:4">
+      <c r="A3256"/>
+    </row>
+    <row r="3257" spans="1:4">
+      <c r="A3257"/>
+    </row>
+    <row r="3258" spans="1:4">
+      <c r="A3258"/>
+    </row>
+    <row r="3259" spans="1:4">
+      <c r="A3259"/>
+    </row>
+    <row r="3260" spans="1:4">
+      <c r="A3260"/>
+    </row>
+    <row r="3261" spans="1:4">
+      <c r="A3261"/>
+    </row>
+    <row r="3262" spans="1:4">
+      <c r="A3262"/>
+    </row>
+    <row r="3263" spans="1:4">
+      <c r="A3263"/>
+    </row>
+    <row r="3264" spans="1:4">
+      <c r="A3264"/>
+    </row>
+    <row r="3265" spans="1:4">
+      <c r="A3265"/>
+    </row>
+    <row r="3266" spans="1:4">
+      <c r="A3266"/>
+    </row>
+    <row r="3267" spans="1:4">
+      <c r="A3267"/>
+    </row>
+    <row r="3268" spans="1:4">
+      <c r="A3268"/>
+    </row>
+    <row r="3269" spans="1:4">
+      <c r="A3269"/>
+    </row>
+    <row r="3270" spans="1:4">
+      <c r="A3270"/>
+    </row>
+    <row r="3271" spans="1:4">
+      <c r="A3271"/>
+    </row>
+    <row r="3272" spans="1:4">
+      <c r="A3272"/>
+    </row>
+    <row r="3273" spans="1:4">
+      <c r="A3273"/>
+    </row>
+    <row r="3274" spans="1:4">
+      <c r="A3274"/>
+    </row>
+    <row r="3275" spans="1:4">
+      <c r="A3275"/>
+    </row>
+    <row r="3276" spans="1:4">
+      <c r="A3276"/>
+    </row>
+    <row r="3277" spans="1:4">
+      <c r="A3277"/>
+    </row>
+    <row r="3278" spans="1:4">
+      <c r="A3278"/>
+    </row>
+    <row r="3279" spans="1:4">
+      <c r="A3279"/>
+    </row>
+    <row r="3280" spans="1:4">
+      <c r="A3280"/>
+    </row>
+    <row r="3281" spans="1:4">
+      <c r="A3281"/>
+    </row>
+    <row r="3282" spans="1:4">
+      <c r="A3282"/>
+    </row>
+    <row r="3283" spans="1:4">
+      <c r="A3283"/>
+    </row>
+    <row r="3284" spans="1:4">
+      <c r="A3284"/>
+    </row>
+    <row r="3285" spans="1:4">
+      <c r="A3285"/>
+    </row>
+    <row r="3286" spans="1:4">
+      <c r="A3286"/>
+    </row>
+    <row r="3287" spans="1:4">
+      <c r="A3287"/>
+    </row>
+    <row r="3288" spans="1:4">
+      <c r="A3288"/>
+    </row>
+    <row r="3289" spans="1:4">
+      <c r="A3289"/>
+    </row>
+    <row r="3290" spans="1:4">
+      <c r="A3290"/>
+    </row>
+    <row r="3291" spans="1:4">
+      <c r="A3291"/>
+    </row>
+    <row r="3292" spans="1:4">
+      <c r="A3292"/>
+    </row>
+    <row r="3293" spans="1:4">
+      <c r="A3293"/>
+    </row>
+    <row r="3294" spans="1:4">
+      <c r="A3294"/>
+    </row>
+    <row r="3295" spans="1:4">
+      <c r="A3295"/>
+    </row>
+    <row r="3296" spans="1:4">
+      <c r="A3296"/>
+    </row>
+    <row r="3297" spans="1:4">
+      <c r="A3297"/>
+    </row>
+    <row r="3298" spans="1:4">
+      <c r="A3298"/>
+    </row>
+    <row r="3299" spans="1:4">
+      <c r="A3299"/>
+    </row>
+    <row r="3300" spans="1:4">
+      <c r="A3300"/>
+    </row>
+    <row r="3301" spans="1:4">
+      <c r="A3301"/>
+    </row>
+    <row r="3302" spans="1:4">
+      <c r="A3302"/>
+    </row>
+    <row r="3303" spans="1:4">
+      <c r="A3303"/>
+    </row>
+    <row r="3304" spans="1:4">
+      <c r="A3304"/>
+    </row>
+    <row r="3305" spans="1:4">
+      <c r="A3305"/>
+    </row>
+    <row r="3306" spans="1:4">
+      <c r="A3306"/>
+    </row>
+    <row r="3307" spans="1:4">
+      <c r="A3307"/>
+    </row>
+    <row r="3308" spans="1:4">
+      <c r="A3308"/>
+    </row>
+    <row r="3309" spans="1:4">
+      <c r="A3309"/>
+    </row>
+    <row r="3310" spans="1:4">
+      <c r="A3310"/>
+    </row>
+    <row r="3311" spans="1:4">
+      <c r="A3311"/>
+    </row>
+    <row r="3312" spans="1:4">
+      <c r="A3312"/>
+    </row>
+    <row r="3313" spans="1:4">
+      <c r="A3313"/>
+    </row>
+    <row r="3314" spans="1:4">
+      <c r="A3314"/>
+    </row>
+    <row r="3315" spans="1:4">
+      <c r="A3315"/>
+    </row>
+    <row r="3316" spans="1:4">
+      <c r="A3316"/>
+    </row>
+    <row r="3317" spans="1:4">
+      <c r="A3317"/>
+    </row>
+    <row r="3318" spans="1:4">
+      <c r="A3318"/>
+    </row>
+    <row r="3319" spans="1:4">
+      <c r="A3319"/>
+    </row>
+    <row r="3320" spans="1:4">
+      <c r="A3320"/>
+    </row>
+    <row r="3321" spans="1:4">
+      <c r="A3321"/>
+    </row>
+    <row r="3322" spans="1:4">
+      <c r="A3322"/>
+    </row>
+    <row r="3323" spans="1:4">
+      <c r="A3323"/>
+    </row>
+    <row r="3324" spans="1:4">
+      <c r="A3324"/>
+    </row>
+    <row r="3325" spans="1:4">
+      <c r="A3325"/>
+    </row>
+    <row r="3326" spans="1:4">
+      <c r="A3326"/>
+    </row>
+    <row r="3327" spans="1:4">
+      <c r="A3327"/>
+    </row>
+    <row r="3328" spans="1:4">
+      <c r="A3328"/>
+    </row>
+    <row r="3329" spans="1:4">
+      <c r="A3329"/>
+    </row>
+    <row r="3330" spans="1:4">
+      <c r="A3330"/>
+    </row>
+    <row r="3331" spans="1:4">
+      <c r="A3331"/>
+    </row>
+    <row r="3332" spans="1:4">
+      <c r="A3332"/>
+    </row>
+    <row r="3333" spans="1:4">
+      <c r="A3333"/>
+    </row>
+    <row r="3334" spans="1:4">
+      <c r="A3334"/>
+    </row>
+    <row r="3335" spans="1:4">
+      <c r="A3335"/>
+    </row>
+    <row r="3336" spans="1:4">
+      <c r="A3336"/>
+    </row>
+    <row r="3337" spans="1:4">
+      <c r="A3337"/>
+    </row>
+    <row r="3338" spans="1:4">
+      <c r="A3338"/>
+    </row>
+    <row r="3339" spans="1:4">
+      <c r="A3339"/>
+    </row>
+    <row r="3340" spans="1:4">
+      <c r="A3340"/>
+    </row>
+    <row r="3341" spans="1:4">
+      <c r="A3341"/>
+    </row>
+    <row r="3342" spans="1:4">
+      <c r="A3342"/>
+    </row>
+    <row r="3343" spans="1:4">
+      <c r="A3343"/>
+    </row>
+    <row r="3344" spans="1:4">
+      <c r="A3344"/>
+    </row>
+    <row r="3345" spans="1:4">
+      <c r="A3345"/>
+    </row>
+    <row r="3346" spans="1:4">
+      <c r="A3346"/>
+    </row>
+    <row r="3347" spans="1:4">
+      <c r="A3347"/>
+    </row>
+    <row r="3348" spans="1:4">
+      <c r="A3348"/>
+    </row>
+    <row r="3349" spans="1:4">
+      <c r="A3349"/>
+    </row>
+    <row r="3350" spans="1:4">
+      <c r="A3350"/>
+    </row>
+    <row r="3351" spans="1:4">
+      <c r="A3351"/>
+    </row>
+    <row r="3352" spans="1:4">
+      <c r="A3352"/>
+    </row>
+    <row r="3353" spans="1:4">
+      <c r="A3353"/>
+    </row>
+    <row r="3354" spans="1:4">
+      <c r="A3354"/>
+    </row>
+    <row r="3355" spans="1:4">
+      <c r="A3355"/>
+    </row>
+    <row r="3356" spans="1:4">
+      <c r="A3356"/>
+    </row>
+    <row r="3357" spans="1:4">
+      <c r="A3357"/>
+    </row>
+    <row r="3358" spans="1:4">
+      <c r="A3358"/>
+    </row>
+    <row r="3359" spans="1:4">
+      <c r="A3359"/>
+    </row>
+    <row r="3360" spans="1:4">
+      <c r="A3360"/>
+    </row>
+    <row r="3361" spans="1:4">
+      <c r="A3361"/>
+    </row>
+    <row r="3362" spans="1:4">
+      <c r="A3362"/>
+    </row>
+    <row r="3363" spans="1:4">
+      <c r="A3363"/>
+    </row>
+    <row r="3364" spans="1:4">
+      <c r="A3364"/>
+    </row>
+    <row r="3365" spans="1:4">
+      <c r="A3365"/>
+    </row>
+    <row r="3366" spans="1:4">
+      <c r="A3366"/>
+    </row>
+    <row r="3367" spans="1:4">
+      <c r="A3367"/>
+    </row>
+    <row r="3368" spans="1:4">
+      <c r="A3368"/>
+    </row>
+    <row r="3369" spans="1:4">
+      <c r="A3369"/>
+    </row>
+    <row r="3370" spans="1:4">
+      <c r="A3370"/>
+    </row>
+    <row r="3371" spans="1:4">
+      <c r="A3371"/>
+    </row>
+    <row r="3372" spans="1:4">
+      <c r="A3372"/>
+    </row>
+    <row r="3373" spans="1:4">
+      <c r="A3373"/>
+    </row>
+    <row r="3374" spans="1:4">
+      <c r="A3374"/>
+    </row>
+    <row r="3375" spans="1:4">
+      <c r="A3375"/>
+    </row>
+    <row r="3376" spans="1:4">
+      <c r="A3376"/>
+    </row>
+    <row r="3377" spans="1:4">
+      <c r="A3377"/>
+    </row>
+    <row r="3378" spans="1:4">
+      <c r="A3378"/>
+    </row>
+    <row r="3379" spans="1:4">
+      <c r="A3379"/>
+    </row>
+    <row r="3380" spans="1:4">
+      <c r="A3380"/>
+    </row>
+    <row r="3381" spans="1:4">
+      <c r="A3381"/>
+    </row>
+    <row r="3382" spans="1:4">
+      <c r="A3382"/>
+    </row>
+    <row r="3383" spans="1:4">
+      <c r="A3383"/>
+    </row>
+    <row r="3384" spans="1:4">
+      <c r="A3384"/>
+    </row>
+    <row r="3385" spans="1:4">
+      <c r="A3385"/>
+    </row>
+    <row r="3386" spans="1:4">
+      <c r="A3386"/>
+    </row>
+    <row r="3387" spans="1:4">
+      <c r="A3387"/>
+    </row>
+    <row r="3388" spans="1:4">
+      <c r="A3388"/>
+    </row>
+    <row r="3389" spans="1:4">
+      <c r="A3389"/>
+    </row>
+    <row r="3390" spans="1:4">
+      <c r="A3390"/>
+    </row>
+    <row r="3391" spans="1:4">
+      <c r="A3391"/>
+    </row>
+    <row r="3392" spans="1:4">
+      <c r="A3392"/>
+    </row>
+    <row r="3393" spans="1:4">
+      <c r="A3393"/>
+    </row>
+    <row r="3394" spans="1:4">
+      <c r="A3394"/>
+    </row>
+    <row r="3395" spans="1:4">
+      <c r="A3395"/>
+    </row>
+    <row r="3396" spans="1:4">
+      <c r="A3396"/>
+    </row>
+    <row r="3397" spans="1:4">
+      <c r="A3397"/>
+    </row>
+    <row r="3398" spans="1:4">
+      <c r="A3398"/>
+    </row>
+    <row r="3399" spans="1:4">
+      <c r="A3399"/>
+    </row>
+    <row r="3400" spans="1:4">
+      <c r="A3400"/>
+    </row>
+    <row r="3401" spans="1:4">
+      <c r="A3401"/>
+    </row>
+    <row r="3402" spans="1:4">
+      <c r="A3402"/>
+    </row>
+    <row r="3403" spans="1:4">
+      <c r="A3403"/>
+    </row>
+    <row r="3404" spans="1:4">
+      <c r="A3404"/>
+    </row>
+    <row r="3405" spans="1:4">
+      <c r="A3405"/>
+    </row>
+    <row r="3406" spans="1:4">
+      <c r="A3406"/>
+    </row>
+    <row r="3407" spans="1:4">
+      <c r="A3407"/>
+    </row>
+    <row r="3408" spans="1:4">
+      <c r="A3408"/>
+    </row>
+    <row r="3409" spans="1:4">
+      <c r="A3409"/>
+    </row>
+    <row r="3410" spans="1:4">
+      <c r="A3410"/>
+    </row>
+    <row r="3411" spans="1:4">
+      <c r="A3411"/>
+    </row>
+    <row r="3412" spans="1:4">
+      <c r="A3412"/>
+    </row>
+    <row r="3413" spans="1:4">
+      <c r="A3413"/>
+    </row>
+    <row r="3414" spans="1:4">
+      <c r="A3414"/>
+    </row>
+    <row r="3415" spans="1:4">
+      <c r="A3415"/>
+    </row>
+    <row r="3416" spans="1:4">
+      <c r="A3416"/>
+    </row>
+    <row r="3417" spans="1:4">
+      <c r="A3417"/>
+    </row>
+    <row r="3418" spans="1:4">
+      <c r="A3418"/>
+    </row>
+    <row r="3419" spans="1:4">
+      <c r="A3419"/>
+    </row>
+    <row r="3420" spans="1:4">
+      <c r="A3420"/>
+    </row>
+    <row r="3421" spans="1:4">
+      <c r="A3421"/>
+    </row>
+    <row r="3422" spans="1:4">
+      <c r="A3422"/>
+    </row>
+    <row r="3423" spans="1:4">
+      <c r="A3423"/>
+    </row>
+    <row r="3424" spans="1:4">
+      <c r="A3424"/>
+    </row>
+    <row r="3425" spans="1:4">
+      <c r="A3425"/>
+    </row>
+    <row r="3426" spans="1:4">
+      <c r="A3426"/>
+    </row>
+    <row r="3427" spans="1:4">
+      <c r="A3427"/>
+    </row>
+    <row r="3428" spans="1:4">
+      <c r="A3428"/>
+    </row>
+    <row r="3429" spans="1:4">
+      <c r="A3429"/>
+    </row>
+    <row r="3430" spans="1:4">
+      <c r="A3430"/>
+    </row>
+    <row r="3431" spans="1:4">
+      <c r="A3431"/>
+    </row>
+    <row r="3432" spans="1:4">
+      <c r="A3432"/>
+    </row>
+    <row r="3433" spans="1:4">
+      <c r="A3433"/>
+    </row>
+    <row r="3434" spans="1:4">
+      <c r="A3434"/>
+    </row>
+    <row r="3435" spans="1:4">
+      <c r="A3435"/>
+    </row>
+    <row r="3436" spans="1:4">
+      <c r="A3436"/>
+    </row>
+    <row r="3437" spans="1:4">
+      <c r="A3437"/>
+    </row>
+    <row r="3438" spans="1:4">
+      <c r="A3438"/>
+    </row>
+    <row r="3439" spans="1:4">
+      <c r="A3439"/>
+    </row>
+    <row r="3440" spans="1:4">
+      <c r="A3440"/>
+    </row>
+    <row r="3441" spans="1:4">
+      <c r="A3441"/>
+    </row>
+    <row r="3442" spans="1:4">
+      <c r="A3442"/>
+    </row>
+    <row r="3443" spans="1:4">
+      <c r="A3443"/>
+    </row>
+    <row r="3444" spans="1:4">
+      <c r="A3444"/>
+    </row>
+    <row r="3445" spans="1:4">
+      <c r="A3445"/>
+    </row>
+    <row r="3446" spans="1:4">
+      <c r="A3446"/>
+    </row>
+    <row r="3447" spans="1:4">
+      <c r="A3447"/>
+    </row>
+    <row r="3448" spans="1:4">
+      <c r="A3448"/>
+    </row>
+    <row r="3449" spans="1:4">
+      <c r="A3449"/>
+    </row>
+    <row r="3450" spans="1:4">
+      <c r="A3450"/>
+    </row>
+    <row r="3451" spans="1:4">
+      <c r="A3451"/>
+    </row>
+    <row r="3452" spans="1:4">
+      <c r="A3452"/>
+    </row>
+    <row r="3453" spans="1:4">
+      <c r="A3453"/>
+    </row>
+    <row r="3454" spans="1:4">
+      <c r="A3454"/>
+    </row>
+    <row r="3455" spans="1:4">
+      <c r="A3455"/>
+    </row>
+    <row r="3456" spans="1:4">
+      <c r="A3456"/>
+    </row>
+    <row r="3457" spans="1:4">
+      <c r="A3457"/>
+    </row>
+    <row r="3458" spans="1:4">
+      <c r="A3458"/>
+    </row>
+    <row r="3459" spans="1:4">
+      <c r="A3459"/>
+    </row>
+    <row r="3460" spans="1:4">
+      <c r="A3460"/>
+    </row>
+    <row r="3461" spans="1:4">
+      <c r="A3461"/>
+    </row>
+    <row r="3462" spans="1:4">
+      <c r="A3462"/>
+    </row>
+    <row r="3463" spans="1:4">
+      <c r="A3463"/>
+    </row>
+    <row r="3464" spans="1:4">
+      <c r="A3464"/>
+    </row>
+    <row r="3465" spans="1:4">
+      <c r="A3465"/>
+    </row>
+    <row r="3466" spans="1:4">
+      <c r="A3466"/>
+    </row>
+    <row r="3467" spans="1:4">
+      <c r="A3467"/>
+    </row>
+    <row r="3468" spans="1:4">
+      <c r="A3468"/>
+    </row>
+    <row r="3469" spans="1:4">
+      <c r="A3469"/>
+    </row>
+    <row r="3470" spans="1:4">
+      <c r="A3470"/>
+    </row>
+    <row r="3471" spans="1:4">
+      <c r="A3471"/>
+    </row>
+    <row r="3472" spans="1:4">
+      <c r="A3472"/>
+    </row>
+    <row r="3473" spans="1:4">
+      <c r="A3473"/>
+    </row>
+    <row r="3474" spans="1:4">
+      <c r="A3474"/>
+    </row>
+    <row r="3475" spans="1:4">
+      <c r="A3475"/>
+    </row>
+    <row r="3476" spans="1:4">
+      <c r="A3476"/>
+    </row>
+    <row r="3477" spans="1:4">
+      <c r="A3477"/>
+    </row>
+    <row r="3478" spans="1:4">
+      <c r="A3478"/>
+    </row>
+    <row r="3479" spans="1:4">
+      <c r="A3479"/>
+    </row>
+    <row r="3480" spans="1:4">
+      <c r="A3480"/>
+    </row>
+    <row r="3481" spans="1:4">
+      <c r="A3481"/>
+    </row>
+    <row r="3482" spans="1:4">
+      <c r="A3482"/>
+    </row>
+    <row r="3483" spans="1:4">
+      <c r="A3483"/>
+    </row>
+    <row r="3484" spans="1:4">
+      <c r="A3484"/>
+    </row>
+    <row r="3485" spans="1:4">
+      <c r="A3485"/>
+    </row>
+    <row r="3486" spans="1:4">
+      <c r="A3486"/>
+    </row>
+    <row r="3487" spans="1:4">
+      <c r="A3487"/>
+    </row>
+    <row r="3488" spans="1:4">
+      <c r="A3488"/>
+    </row>
+    <row r="3489" spans="1:4">
+      <c r="A3489"/>
+    </row>
+    <row r="3490" spans="1:4">
+      <c r="A3490"/>
+    </row>
+    <row r="3491" spans="1:4">
+      <c r="A3491"/>
+    </row>
+    <row r="3492" spans="1:4">
+      <c r="A3492"/>
+    </row>
+    <row r="3493" spans="1:4">
+      <c r="A3493"/>
+    </row>
+    <row r="3494" spans="1:4">
+      <c r="A3494"/>
+    </row>
+    <row r="3495" spans="1:4">
+      <c r="A3495"/>
+    </row>
+    <row r="3496" spans="1:4">
+      <c r="A3496"/>
+    </row>
+    <row r="3497" spans="1:4">
+      <c r="A3497"/>
+    </row>
+    <row r="3498" spans="1:4">
+      <c r="A3498"/>
+    </row>
+    <row r="3499" spans="1:4">
+      <c r="A3499"/>
+    </row>
+    <row r="3500" spans="1:4">
+      <c r="A3500"/>
+    </row>
+    <row r="3501" spans="1:4">
+      <c r="A3501"/>
+    </row>
+    <row r="3502" spans="1:4">
+      <c r="A3502"/>
+    </row>
+    <row r="3503" spans="1:4">
+      <c r="A3503"/>
+    </row>
+    <row r="3504" spans="1:4">
+      <c r="A3504"/>
+    </row>
+    <row r="3505" spans="1:4">
+      <c r="A3505"/>
+    </row>
+    <row r="3506" spans="1:4">
+      <c r="A3506"/>
+    </row>
+    <row r="3507" spans="1:4">
+      <c r="A3507"/>
+    </row>
+    <row r="3508" spans="1:4">
+      <c r="A3508"/>
+    </row>
+    <row r="3509" spans="1:4">
+      <c r="A3509"/>
+    </row>
+    <row r="3510" spans="1:4">
+      <c r="A3510"/>
+    </row>
+    <row r="3511" spans="1:4">
+      <c r="A3511"/>
+    </row>
+    <row r="3512" spans="1:4">
+      <c r="A3512"/>
+    </row>
+    <row r="3513" spans="1:4">
+      <c r="A3513"/>
+    </row>
+    <row r="3514" spans="1:4">
+      <c r="A3514"/>
+    </row>
+    <row r="3515" spans="1:4">
+      <c r="A3515"/>
+    </row>
+    <row r="3516" spans="1:4">
+      <c r="A3516"/>
+    </row>
+    <row r="3517" spans="1:4">
+      <c r="A3517"/>
+    </row>
+    <row r="3518" spans="1:4">
+      <c r="A3518"/>
+    </row>
+    <row r="3519" spans="1:4">
+      <c r="A3519"/>
+    </row>
+    <row r="3520" spans="1:4">
+      <c r="A3520"/>
+    </row>
+    <row r="3521" spans="1:4">
+      <c r="A3521"/>
+    </row>
+    <row r="3522" spans="1:4">
+      <c r="A3522"/>
+    </row>
+    <row r="3523" spans="1:4">
+      <c r="A3523"/>
+    </row>
+    <row r="3524" spans="1:4">
+      <c r="A3524"/>
+    </row>
+    <row r="3525" spans="1:4">
+      <c r="A3525"/>
+    </row>
+    <row r="3526" spans="1:4">
+      <c r="A3526"/>
+    </row>
+    <row r="3527" spans="1:4">
+      <c r="A3527"/>
+    </row>
+    <row r="3528" spans="1:4">
+      <c r="A3528"/>
+    </row>
+    <row r="3529" spans="1:4">
+      <c r="A3529"/>
+    </row>
+    <row r="3530" spans="1:4">
+      <c r="A3530"/>
+    </row>
+    <row r="3531" spans="1:4">
+      <c r="A3531"/>
+    </row>
+    <row r="3532" spans="1:4">
+      <c r="A3532"/>
+    </row>
+    <row r="3533" spans="1:4">
+      <c r="A3533"/>
+    </row>
+    <row r="3534" spans="1:4">
+      <c r="A3534"/>
+    </row>
+    <row r="3535" spans="1:4">
+      <c r="A3535"/>
+    </row>
+    <row r="3536" spans="1:4">
+      <c r="A3536"/>
+    </row>
+    <row r="3537" spans="1:4">
+      <c r="A3537"/>
+    </row>
+    <row r="3538" spans="1:4">
+      <c r="A3538"/>
+    </row>
+    <row r="3539" spans="1:4">
+      <c r="A3539"/>
+    </row>
+    <row r="3540" spans="1:4">
+      <c r="A3540"/>
+    </row>
+    <row r="3541" spans="1:4">
+      <c r="A3541"/>
+    </row>
+    <row r="3542" spans="1:4">
+      <c r="A3542"/>
+    </row>
+    <row r="3543" spans="1:4">
+      <c r="A3543"/>
+    </row>
+    <row r="3544" spans="1:4">
+      <c r="A3544"/>
+    </row>
+    <row r="3545" spans="1:4">
+      <c r="A3545"/>
+    </row>
+    <row r="3546" spans="1:4">
+      <c r="A3546"/>
+    </row>
+    <row r="3547" spans="1:4">
+      <c r="A3547"/>
+    </row>
+    <row r="3548" spans="1:4">
+      <c r="A3548"/>
+    </row>
+    <row r="3549" spans="1:4">
+      <c r="A3549"/>
+    </row>
+    <row r="3550" spans="1:4">
+      <c r="A3550"/>
+    </row>
+    <row r="3551" spans="1:4">
+      <c r="A3551"/>
+    </row>
+    <row r="3552" spans="1:4">
+      <c r="A3552"/>
+    </row>
+    <row r="3553" spans="1:4">
+      <c r="A3553"/>
+    </row>
+    <row r="3554" spans="1:4">
+      <c r="A3554"/>
+    </row>
+    <row r="3555" spans="1:4">
+      <c r="A3555"/>
+    </row>
+    <row r="3556" spans="1:4">
+      <c r="A3556"/>
+    </row>
+    <row r="3557" spans="1:4">
+      <c r="A3557"/>
+    </row>
+    <row r="3558" spans="1:4">
+      <c r="A3558"/>
+    </row>
+    <row r="3559" spans="1:4">
+      <c r="A3559"/>
+    </row>
+    <row r="3560" spans="1:4">
+      <c r="A3560"/>
+    </row>
+    <row r="3561" spans="1:4">
+      <c r="A3561"/>
+    </row>
+    <row r="3562" spans="1:4">
+      <c r="A3562"/>
+    </row>
+    <row r="3563" spans="1:4">
+      <c r="A3563"/>
+    </row>
+    <row r="3564" spans="1:4">
+      <c r="A3564"/>
+    </row>
+    <row r="3565" spans="1:4">
+      <c r="A3565"/>
+    </row>
+    <row r="3566" spans="1:4">
+      <c r="A3566"/>
+    </row>
+    <row r="3567" spans="1:4">
+      <c r="A3567"/>
+    </row>
+    <row r="3568" spans="1:4">
+      <c r="A3568"/>
+    </row>
+    <row r="3569" spans="1:4">
+      <c r="A3569"/>
+    </row>
+    <row r="3570" spans="1:4">
+      <c r="A3570"/>
+    </row>
+    <row r="3571" spans="1:4">
+      <c r="A3571"/>
+    </row>
+    <row r="3572" spans="1:4">
+      <c r="A3572"/>
+    </row>
+    <row r="3573" spans="1:4">
+      <c r="A3573"/>
+    </row>
+    <row r="3574" spans="1:4">
+      <c r="A3574"/>
+    </row>
+    <row r="3575" spans="1:4">
+      <c r="A3575"/>
+    </row>
+    <row r="3576" spans="1:4">
+      <c r="A3576"/>
+    </row>
+    <row r="3577" spans="1:4">
+      <c r="A3577"/>
+    </row>
+    <row r="3578" spans="1:4">
+      <c r="A3578"/>
+    </row>
+    <row r="3579" spans="1:4">
+      <c r="A3579"/>
+    </row>
+    <row r="3580" spans="1:4">
+      <c r="A3580"/>
+    </row>
+    <row r="3581" spans="1:4">
+      <c r="A3581"/>
+    </row>
+    <row r="3582" spans="1:4">
+      <c r="A3582"/>
+    </row>
+    <row r="3583" spans="1:4">
+      <c r="A3583"/>
+    </row>
+    <row r="3584" spans="1:4">
+      <c r="A3584"/>
+    </row>
+    <row r="3585" spans="1:4">
+      <c r="A3585"/>
+    </row>
+    <row r="3586" spans="1:4">
+      <c r="A3586"/>
+    </row>
+    <row r="3587" spans="1:4">
+      <c r="A3587"/>
+    </row>
+    <row r="3588" spans="1:4">
+      <c r="A3588"/>
+    </row>
+    <row r="3589" spans="1:4">
+      <c r="A3589"/>
+    </row>
+    <row r="3590" spans="1:4">
+      <c r="A3590"/>
+    </row>
+    <row r="3591" spans="1:4">
+      <c r="A3591"/>
+    </row>
+    <row r="3592" spans="1:4">
+      <c r="A3592"/>
+    </row>
+    <row r="3593" spans="1:4">
+      <c r="A3593"/>
+    </row>
+    <row r="3594" spans="1:4">
+      <c r="A3594"/>
+    </row>
+    <row r="3595" spans="1:4">
+      <c r="A3595"/>
+    </row>
+    <row r="3596" spans="1:4">
+      <c r="A3596"/>
+    </row>
+    <row r="3597" spans="1:4">
+      <c r="A3597"/>
+    </row>
+    <row r="3598" spans="1:4">
+      <c r="A3598"/>
+    </row>
+    <row r="3599" spans="1:4">
+      <c r="A3599"/>
+    </row>
+    <row r="3600" spans="1:4">
+      <c r="A3600"/>
+    </row>
+    <row r="3601" spans="1:4">
+      <c r="A3601"/>
+    </row>
+    <row r="3602" spans="1:4">
+      <c r="A3602"/>
+    </row>
+    <row r="3603" spans="1:4">
+      <c r="A3603"/>
+    </row>
+    <row r="3604" spans="1:4">
+      <c r="A3604"/>
+    </row>
+    <row r="3605" spans="1:4">
+      <c r="A3605"/>
+    </row>
+    <row r="3606" spans="1:4">
+      <c r="A3606"/>
+    </row>
+    <row r="3607" spans="1:4">
+      <c r="A3607"/>
+    </row>
+    <row r="3608" spans="1:4">
+      <c r="A3608"/>
+    </row>
+    <row r="3609" spans="1:4">
+      <c r="A3609"/>
+    </row>
+    <row r="3610" spans="1:4">
+      <c r="A3610"/>
+    </row>
+    <row r="3611" spans="1:4">
+      <c r="A3611"/>
+    </row>
+    <row r="3612" spans="1:4">
+      <c r="A3612"/>
+    </row>
+    <row r="3613" spans="1:4">
+      <c r="A3613"/>
+    </row>
+    <row r="3614" spans="1:4">
+      <c r="A3614"/>
+    </row>
+    <row r="3615" spans="1:4">
+      <c r="A3615"/>
+    </row>
+    <row r="3616" spans="1:4">
+      <c r="A3616"/>
+    </row>
+    <row r="3617" spans="1:4">
+      <c r="A3617"/>
+    </row>
+    <row r="3618" spans="1:4">
+      <c r="A3618"/>
+    </row>
+    <row r="3619" spans="1:4">
+      <c r="A3619"/>
+    </row>
+    <row r="3620" spans="1:4">
+      <c r="A3620"/>
+    </row>
+    <row r="3621" spans="1:4">
+      <c r="A3621"/>
+    </row>
+    <row r="3622" spans="1:4">
+      <c r="A3622"/>
+    </row>
+    <row r="3623" spans="1:4">
+      <c r="A3623"/>
+    </row>
+    <row r="3624" spans="1:4">
+      <c r="A3624"/>
+    </row>
+    <row r="3625" spans="1:4">
+      <c r="A3625"/>
+    </row>
+    <row r="3626" spans="1:4">
+      <c r="A3626"/>
+    </row>
+    <row r="3627" spans="1:4">
+      <c r="A3627"/>
+    </row>
+    <row r="3628" spans="1:4">
+      <c r="A3628"/>
+    </row>
+    <row r="3629" spans="1:4">
+      <c r="A3629"/>
+    </row>
+    <row r="3630" spans="1:4">
+      <c r="A3630"/>
+    </row>
+    <row r="3631" spans="1:4">
+      <c r="A3631"/>
+    </row>
+    <row r="3632" spans="1:4">
+      <c r="A3632"/>
+    </row>
+    <row r="3633" spans="1:4">
+      <c r="A3633"/>
+    </row>
+    <row r="3634" spans="1:4">
+      <c r="A3634"/>
+    </row>
+    <row r="3635" spans="1:4">
+      <c r="A3635"/>
+    </row>
+    <row r="3636" spans="1:4">
+      <c r="A3636"/>
+    </row>
+    <row r="3637" spans="1:4">
+      <c r="A3637"/>
+    </row>
+    <row r="3638" spans="1:4">
+      <c r="A3638"/>
+    </row>
+    <row r="3639" spans="1:4">
+      <c r="A3639"/>
+    </row>
+    <row r="3640" spans="1:4">
+      <c r="A3640"/>
+    </row>
+    <row r="3641" spans="1:4">
+      <c r="A3641"/>
+    </row>
+    <row r="3642" spans="1:4">
+      <c r="A3642"/>
+    </row>
+    <row r="3643" spans="1:4">
+      <c r="A3643"/>
+    </row>
+    <row r="3644" spans="1:4">
+      <c r="A3644"/>
+    </row>
+    <row r="3645" spans="1:4">
+      <c r="A3645"/>
+    </row>
+    <row r="3646" spans="1:4">
+      <c r="A3646"/>
+    </row>
+    <row r="3647" spans="1:4">
+      <c r="A3647"/>
+    </row>
+    <row r="3648" spans="1:4">
+      <c r="A3648"/>
+    </row>
+    <row r="3649" spans="1:4">
+      <c r="A3649"/>
+    </row>
+    <row r="3650" spans="1:4">
+      <c r="A3650"/>
+    </row>
+    <row r="3651" spans="1:4">
+      <c r="A3651"/>
+    </row>
+    <row r="3652" spans="1:4">
+      <c r="A3652"/>
+    </row>
+    <row r="3653" spans="1:4">
+      <c r="A3653"/>
+    </row>
+    <row r="3654" spans="1:4">
+      <c r="A3654"/>
+    </row>
+    <row r="3655" spans="1:4">
+      <c r="A3655"/>
+    </row>
+    <row r="3656" spans="1:4">
+      <c r="A3656"/>
+    </row>
+    <row r="3657" spans="1:4">
+      <c r="A3657"/>
+    </row>
+    <row r="3658" spans="1:4">
+      <c r="A3658"/>
+    </row>
+    <row r="3659" spans="1:4">
+      <c r="A3659"/>
+    </row>
+    <row r="3660" spans="1:4">
+      <c r="A3660"/>
+    </row>
+    <row r="3661" spans="1:4">
+      <c r="A3661"/>
+    </row>
+    <row r="3662" spans="1:4">
+      <c r="A3662"/>
+    </row>
+    <row r="3663" spans="1:4">
+      <c r="A3663"/>
+    </row>
+    <row r="3664" spans="1:4">
+      <c r="A3664"/>
+    </row>
+    <row r="3665" spans="1:4">
+      <c r="A3665"/>
+    </row>
+    <row r="3666" spans="1:4">
+      <c r="A3666"/>
+    </row>
+    <row r="3667" spans="1:4">
+      <c r="A3667"/>
+    </row>
+    <row r="3668" spans="1:4">
+      <c r="A3668"/>
+    </row>
+    <row r="3669" spans="1:4">
+      <c r="A3669"/>
+    </row>
+    <row r="3670" spans="1:4">
+      <c r="A3670"/>
+    </row>
+    <row r="3671" spans="1:4">
+      <c r="A3671"/>
+    </row>
+    <row r="3672" spans="1:4">
+      <c r="A3672"/>
+    </row>
+    <row r="3673" spans="1:4">
+      <c r="A3673"/>
+    </row>
+    <row r="3674" spans="1:4">
+      <c r="A3674"/>
+    </row>
+    <row r="3675" spans="1:4">
+      <c r="A3675"/>
+    </row>
+    <row r="3676" spans="1:4">
+      <c r="A3676"/>
+    </row>
+    <row r="3677" spans="1:4">
+      <c r="A3677"/>
+    </row>
+    <row r="3678" spans="1:4">
+      <c r="A3678"/>
+    </row>
+    <row r="3679" spans="1:4">
+      <c r="A3679"/>
+    </row>
+    <row r="3680" spans="1:4">
+      <c r="A3680"/>
+    </row>
+    <row r="3681" spans="1:4">
+      <c r="A3681"/>
+    </row>
+    <row r="3682" spans="1:4">
+      <c r="A3682"/>
+    </row>
+    <row r="3683" spans="1:4">
+      <c r="A3683"/>
+    </row>
+    <row r="3684" spans="1:4">
+      <c r="A3684"/>
+    </row>
+    <row r="3685" spans="1:4">
+      <c r="A3685"/>
+    </row>
+    <row r="3686" spans="1:4">
+      <c r="A3686"/>
+    </row>
+    <row r="3687" spans="1:4">
+      <c r="A3687"/>
+    </row>
+    <row r="3688" spans="1:4">
+      <c r="A3688"/>
+    </row>
+    <row r="3689" spans="1:4">
+      <c r="A3689"/>
+    </row>
+    <row r="3690" spans="1:4">
+      <c r="A3690"/>
+    </row>
+    <row r="3691" spans="1:4">
+      <c r="A3691"/>
+    </row>
+    <row r="3692" spans="1:4">
+      <c r="A3692"/>
+    </row>
+    <row r="3693" spans="1:4">
+      <c r="A3693"/>
+    </row>
+    <row r="3694" spans="1:4">
+      <c r="A3694"/>
+    </row>
+    <row r="3695" spans="1:4">
+      <c r="A3695"/>
+    </row>
+    <row r="3696" spans="1:4">
+      <c r="A3696"/>
+    </row>
+    <row r="3697" spans="1:4">
+      <c r="A3697"/>
+    </row>
+    <row r="3698" spans="1:4">
+      <c r="A3698"/>
+    </row>
+    <row r="3699" spans="1:4">
+      <c r="A3699"/>
+    </row>
+    <row r="3700" spans="1:4">
+      <c r="A3700"/>
+    </row>
+    <row r="3701" spans="1:4">
+      <c r="A3701"/>
+    </row>
+    <row r="3702" spans="1:4">
+      <c r="A3702"/>
+    </row>
+    <row r="3703" spans="1:4">
+      <c r="A3703"/>
+    </row>
+    <row r="3704" spans="1:4">
+      <c r="A3704"/>
+    </row>
+    <row r="3705" spans="1:4">
+      <c r="A3705"/>
+    </row>
+    <row r="3706" spans="1:4">
+      <c r="A3706"/>
+    </row>
+    <row r="3707" spans="1:4">
+      <c r="A3707"/>
+    </row>
+    <row r="3708" spans="1:4">
+      <c r="A3708"/>
+    </row>
+    <row r="3709" spans="1:4">
+      <c r="A3709"/>
+    </row>
+    <row r="3710" spans="1:4">
+      <c r="A3710"/>
+    </row>
+    <row r="3711" spans="1:4">
+      <c r="A3711"/>
+    </row>
+    <row r="3712" spans="1:4">
+      <c r="A3712"/>
+    </row>
+    <row r="3713" spans="1:4">
+      <c r="A3713"/>
+    </row>
+    <row r="3714" spans="1:4">
+      <c r="A3714"/>
+    </row>
+    <row r="3715" spans="1:4">
+      <c r="A3715"/>
+    </row>
+    <row r="3716" spans="1:4">
+      <c r="A3716"/>
+    </row>
+    <row r="3717" spans="1:4">
+      <c r="A3717"/>
+    </row>
+    <row r="3718" spans="1:4">
+      <c r="A3718"/>
+    </row>
+    <row r="3719" spans="1:4">
+      <c r="A3719"/>
+    </row>
+    <row r="3720" spans="1:4">
+      <c r="A3720"/>
+    </row>
+    <row r="3721" spans="1:4">
+      <c r="A3721"/>
+    </row>
+    <row r="3722" spans="1:4">
+      <c r="A3722"/>
+    </row>
+    <row r="3723" spans="1:4">
+      <c r="A3723"/>
+    </row>
+    <row r="3724" spans="1:4">
+      <c r="A3724"/>
+    </row>
+    <row r="3725" spans="1:4">
+      <c r="A3725"/>
+    </row>
+    <row r="3726" spans="1:4">
+      <c r="A3726"/>
+    </row>
+    <row r="3727" spans="1:4">
+      <c r="A3727"/>
+    </row>
+    <row r="3728" spans="1:4">
+      <c r="A3728"/>
+    </row>
+    <row r="3729" spans="1:4">
+      <c r="A3729"/>
+    </row>
+    <row r="3730" spans="1:4">
+      <c r="A3730"/>
+    </row>
+    <row r="3731" spans="1:4">
+      <c r="A3731"/>
+    </row>
+    <row r="3732" spans="1:4">
+      <c r="A3732"/>
+    </row>
+    <row r="3733" spans="1:4">
+      <c r="A3733"/>
+    </row>
+    <row r="3734" spans="1:4">
+      <c r="A3734"/>
+    </row>
+    <row r="3735" spans="1:4">
+      <c r="A3735"/>
+    </row>
+    <row r="3736" spans="1:4">
+      <c r="A3736"/>
+    </row>
+    <row r="3737" spans="1:4">
+      <c r="A3737"/>
+    </row>
+    <row r="3738" spans="1:4">
+      <c r="A3738"/>
+    </row>
+    <row r="3739" spans="1:4">
+      <c r="A3739"/>
+    </row>
+    <row r="3740" spans="1:4">
+      <c r="A3740"/>
+    </row>
+    <row r="3741" spans="1:4">
+      <c r="A3741"/>
+    </row>
+    <row r="3742" spans="1:4">
+      <c r="A3742"/>
+    </row>
+    <row r="3743" spans="1:4">
+      <c r="A3743"/>
+    </row>
+    <row r="3744" spans="1:4">
+      <c r="A3744"/>
+    </row>
+    <row r="3745" spans="1:4">
+      <c r="A3745"/>
+    </row>
+    <row r="3746" spans="1:4">
+      <c r="A3746"/>
+    </row>
+    <row r="3747" spans="1:4">
+      <c r="A3747"/>
+    </row>
+    <row r="3748" spans="1:4">
+      <c r="A3748"/>
+    </row>
+    <row r="3749" spans="1:4">
+      <c r="A3749"/>
+    </row>
+    <row r="3750" spans="1:4">
+      <c r="A3750"/>
+    </row>
+    <row r="3751" spans="1:4">
+      <c r="A3751"/>
+    </row>
+    <row r="3752" spans="1:4">
+      <c r="A3752"/>
+    </row>
+    <row r="3753" spans="1:4">
+      <c r="A3753"/>
+    </row>
+    <row r="3754" spans="1:4">
+      <c r="A3754"/>
+    </row>
+    <row r="3755" spans="1:4">
+      <c r="A3755"/>
+    </row>
+    <row r="3756" spans="1:4">
+      <c r="A3756"/>
+    </row>
+    <row r="3757" spans="1:4">
+      <c r="A3757"/>
+    </row>
+    <row r="3758" spans="1:4">
+      <c r="A3758"/>
+    </row>
+    <row r="3759" spans="1:4">
+      <c r="A3759"/>
+    </row>
+    <row r="3760" spans="1:4">
+      <c r="A3760"/>
+    </row>
+    <row r="3761" spans="1:4">
+      <c r="A3761"/>
+    </row>
+    <row r="3762" spans="1:4">
+      <c r="A3762"/>
+    </row>
+    <row r="3763" spans="1:4">
+      <c r="A3763"/>
+    </row>
+    <row r="3764" spans="1:4">
+      <c r="A3764"/>
+    </row>
+    <row r="3765" spans="1:4">
+      <c r="A3765"/>
+    </row>
+    <row r="3766" spans="1:4">
+      <c r="A3766"/>
+    </row>
+    <row r="3767" spans="1:4">
+      <c r="A3767"/>
+    </row>
+    <row r="3768" spans="1:4">
+      <c r="A3768"/>
+    </row>
+    <row r="3769" spans="1:4">
+      <c r="A3769"/>
+    </row>
+    <row r="3770" spans="1:4">
+      <c r="A3770"/>
+    </row>
+    <row r="3771" spans="1:4">
+      <c r="A3771"/>
+    </row>
+    <row r="3772" spans="1:4">
+      <c r="A3772"/>
+    </row>
+    <row r="3773" spans="1:4">
+      <c r="A3773"/>
+    </row>
+    <row r="3774" spans="1:4">
+      <c r="A3774"/>
+    </row>
+    <row r="3775" spans="1:4">
+      <c r="A3775"/>
+    </row>
+    <row r="3776" spans="1:4">
+      <c r="A3776"/>
+    </row>
+    <row r="3777" spans="1:4">
+      <c r="A3777"/>
+    </row>
+    <row r="3778" spans="1:4">
+      <c r="A3778"/>
+    </row>
+    <row r="3779" spans="1:4">
+      <c r="A3779"/>
+    </row>
+    <row r="3780" spans="1:4">
+      <c r="A3780"/>
+    </row>
+    <row r="3781" spans="1:4">
+      <c r="A3781"/>
+    </row>
+    <row r="3782" spans="1:4">
+      <c r="A3782"/>
+    </row>
+    <row r="3783" spans="1:4">
+      <c r="A3783"/>
+    </row>
+    <row r="3784" spans="1:4">
+      <c r="A3784"/>
+    </row>
+    <row r="3785" spans="1:4">
+      <c r="A3785"/>
+    </row>
+    <row r="3786" spans="1:4">
+      <c r="A3786"/>
+    </row>
+    <row r="3787" spans="1:4">
+      <c r="A3787"/>
+    </row>
+    <row r="3788" spans="1:4">
+      <c r="A3788"/>
+    </row>
+    <row r="3789" spans="1:4">
+      <c r="A3789"/>
+    </row>
+    <row r="3790" spans="1:4">
+      <c r="A3790"/>
+    </row>
+    <row r="3791" spans="1:4">
+      <c r="A3791"/>
+    </row>
+    <row r="3792" spans="1:4">
+      <c r="A3792"/>
+    </row>
+    <row r="3793" spans="1:4">
+      <c r="A3793"/>
+    </row>
+    <row r="3794" spans="1:4">
+      <c r="A3794"/>
+    </row>
+    <row r="3795" spans="1:4">
+      <c r="A3795"/>
+    </row>
+    <row r="3796" spans="1:4">
+      <c r="A3796"/>
+    </row>
+    <row r="3797" spans="1:4">
+      <c r="A3797"/>
+    </row>
+    <row r="3798" spans="1:4">
+      <c r="A3798"/>
+    </row>
+    <row r="3799" spans="1:4">
+      <c r="A3799"/>
+    </row>
+    <row r="3800" spans="1:4">
+      <c r="A3800"/>
+    </row>
+    <row r="3801" spans="1:4">
+      <c r="A3801"/>
+    </row>
+    <row r="3802" spans="1:4">
+      <c r="A3802"/>
+    </row>
+    <row r="3803" spans="1:4">
+      <c r="A3803"/>
+    </row>
+    <row r="3804" spans="1:4">
+      <c r="A3804"/>
+    </row>
+    <row r="3805" spans="1:4">
+      <c r="A3805"/>
+    </row>
+    <row r="3806" spans="1:4">
+      <c r="A3806"/>
+    </row>
+    <row r="3807" spans="1:4">
+      <c r="A3807"/>
+    </row>
+    <row r="3808" spans="1:4">
+      <c r="A3808"/>
+    </row>
+    <row r="3809" spans="1:4">
+      <c r="A3809"/>
+    </row>
+    <row r="3810" spans="1:4">
+      <c r="A3810"/>
+    </row>
+    <row r="3811" spans="1:4">
+      <c r="A3811"/>
+    </row>
+    <row r="3812" spans="1:4">
+      <c r="A3812"/>
+    </row>
+    <row r="3813" spans="1:4">
+      <c r="A3813"/>
+    </row>
+    <row r="3814" spans="1:4">
+      <c r="A3814"/>
+    </row>
+    <row r="3815" spans="1:4">
+      <c r="A3815"/>
+    </row>
+    <row r="3816" spans="1:4">
+      <c r="A3816"/>
+    </row>
+    <row r="3817" spans="1:4">
+      <c r="A3817"/>
+    </row>
+    <row r="3818" spans="1:4">
+      <c r="A3818"/>
+    </row>
+    <row r="3819" spans="1:4">
+      <c r="A3819"/>
+    </row>
+    <row r="3820" spans="1:4">
+      <c r="A3820"/>
+    </row>
+    <row r="3821" spans="1:4">
+      <c r="A3821"/>
+    </row>
+    <row r="3822" spans="1:4">
+      <c r="A3822"/>
+    </row>
+    <row r="3823" spans="1:4">
+      <c r="A3823"/>
+    </row>
+    <row r="3824" spans="1:4">
+      <c r="A3824"/>
+    </row>
+    <row r="3825" spans="1:4">
+      <c r="A3825"/>
+    </row>
+    <row r="3826" spans="1:4">
+      <c r="A3826"/>
+    </row>
+    <row r="3827" spans="1:4">
+      <c r="A3827"/>
+    </row>
+    <row r="3828" spans="1:4">
+      <c r="A3828"/>
+    </row>
+    <row r="3829" spans="1:4">
+      <c r="A3829"/>
+    </row>
+    <row r="3830" spans="1:4">
+      <c r="A3830"/>
+    </row>
+    <row r="3831" spans="1:4">
+      <c r="A3831"/>
+    </row>
+    <row r="3832" spans="1:4">
+      <c r="A3832"/>
+    </row>
+    <row r="3833" spans="1:4">
+      <c r="A3833"/>
+    </row>
+    <row r="3834" spans="1:4">
+      <c r="A3834"/>
+    </row>
+    <row r="3835" spans="1:4">
+      <c r="A3835"/>
+    </row>
+    <row r="3836" spans="1:4">
+      <c r="A3836"/>
+    </row>
+    <row r="3837" spans="1:4">
+      <c r="A3837"/>
+    </row>
+    <row r="3838" spans="1:4">
+      <c r="A3838"/>
+    </row>
+    <row r="3839" spans="1:4">
+      <c r="A3839"/>
+    </row>
+    <row r="3840" spans="1:4">
+      <c r="A3840"/>
+    </row>
+    <row r="3841" spans="1:4">
+      <c r="A3841"/>
+    </row>
+    <row r="3842" spans="1:4">
+      <c r="A3842"/>
+    </row>
+    <row r="3843" spans="1:4">
+      <c r="A3843"/>
+    </row>
+    <row r="3844" spans="1:4">
+      <c r="A3844"/>
+    </row>
+    <row r="3845" spans="1:4">
+      <c r="A3845"/>
+    </row>
+    <row r="3846" spans="1:4">
+      <c r="A3846"/>
+    </row>
+    <row r="3847" spans="1:4">
+      <c r="A3847"/>
+    </row>
+    <row r="3848" spans="1:4">
+      <c r="A3848"/>
+    </row>
+    <row r="3849" spans="1:4">
+      <c r="A3849"/>
+    </row>
+    <row r="3850" spans="1:4">
+      <c r="A3850"/>
+    </row>
+    <row r="3851" spans="1:4">
+      <c r="A3851"/>
+    </row>
+    <row r="3852" spans="1:4">
+      <c r="A3852"/>
+    </row>
+    <row r="3853" spans="1:4">
+      <c r="A3853"/>
+    </row>
+    <row r="3854" spans="1:4">
+      <c r="A3854"/>
+    </row>
+    <row r="3855" spans="1:4">
+      <c r="A3855"/>
+    </row>
+    <row r="3856" spans="1:4">
+      <c r="A3856"/>
+    </row>
+    <row r="3857" spans="1:4">
+      <c r="A3857"/>
+    </row>
+    <row r="3858" spans="1:4">
+      <c r="A3858"/>
+    </row>
+    <row r="3859" spans="1:4">
+      <c r="A3859"/>
+    </row>
+    <row r="3860" spans="1:4">
+      <c r="A3860"/>
+    </row>
+    <row r="3861" spans="1:4">
+      <c r="A3861"/>
+    </row>
+    <row r="3862" spans="1:4">
+      <c r="A3862"/>
+    </row>
+    <row r="3863" spans="1:4">
+      <c r="A3863"/>
+    </row>
+    <row r="3864" spans="1:4">
+      <c r="A3864"/>
+    </row>
+    <row r="3865" spans="1:4">
+      <c r="A3865"/>
+    </row>
+    <row r="3866" spans="1:4">
+      <c r="A3866"/>
+    </row>
+    <row r="3867" spans="1:4">
+      <c r="A3867"/>
+    </row>
+    <row r="3868" spans="1:4">
+      <c r="A3868"/>
+    </row>
+    <row r="3869" spans="1:4">
+      <c r="A3869"/>
+    </row>
+    <row r="3870" spans="1:4">
+      <c r="A3870"/>
+    </row>
+    <row r="3871" spans="1:4">
+      <c r="A3871"/>
+    </row>
+    <row r="3872" spans="1:4">
+      <c r="A3872"/>
+    </row>
+    <row r="3873" spans="1:4">
+      <c r="A3873"/>
+    </row>
+    <row r="3874" spans="1:4">
+      <c r="A3874"/>
+    </row>
+    <row r="3875" spans="1:4">
+      <c r="A3875"/>
+    </row>
+    <row r="3876" spans="1:4">
+      <c r="A3876"/>
+    </row>
+    <row r="3877" spans="1:4">
+      <c r="A3877"/>
+    </row>
+    <row r="3878" spans="1:4">
+      <c r="A3878"/>
+    </row>
+    <row r="3879" spans="1:4">
+      <c r="A3879"/>
+    </row>
+    <row r="3880" spans="1:4">
+      <c r="A3880"/>
+    </row>
+    <row r="3881" spans="1:4">
+      <c r="A3881"/>
+    </row>
+    <row r="3882" spans="1:4">
+      <c r="A3882"/>
+    </row>
+    <row r="3883" spans="1:4">
+      <c r="A3883"/>
+    </row>
+    <row r="3884" spans="1:4">
+      <c r="A3884"/>
+    </row>
+    <row r="3885" spans="1:4">
+      <c r="A3885"/>
+    </row>
+    <row r="3886" spans="1:4">
+      <c r="A3886"/>
+    </row>
+    <row r="3887" spans="1:4">
+      <c r="A3887"/>
+    </row>
+    <row r="3888" spans="1:4">
+      <c r="A3888"/>
+    </row>
+    <row r="3889" spans="1:4">
+      <c r="A3889"/>
+    </row>
+    <row r="3890" spans="1:4">
+      <c r="A3890"/>
+    </row>
+    <row r="3891" spans="1:4">
+      <c r="A3891"/>
+    </row>
+    <row r="3892" spans="1:4">
+      <c r="A3892"/>
+    </row>
+    <row r="3893" spans="1:4">
+      <c r="A3893"/>
+    </row>
+    <row r="3894" spans="1:4">
+      <c r="A3894"/>
+    </row>
+    <row r="3895" spans="1:4">
+      <c r="A3895"/>
+    </row>
+    <row r="3896" spans="1:4">
+      <c r="A3896"/>
+    </row>
+    <row r="3897" spans="1:4">
+      <c r="A3897"/>
+    </row>
+    <row r="3898" spans="1:4">
+      <c r="A3898"/>
+    </row>
+    <row r="3899" spans="1:4">
+      <c r="A3899"/>
+    </row>
+    <row r="3900" spans="1:4">
+      <c r="A3900"/>
+    </row>
+    <row r="3901" spans="1:4">
+      <c r="A3901"/>
+    </row>
+    <row r="3902" spans="1:4">
+      <c r="A3902"/>
+    </row>
+    <row r="3903" spans="1:4">
+      <c r="A3903"/>
+    </row>
+    <row r="3904" spans="1:4">
+      <c r="A3904"/>
+    </row>
+    <row r="3905" spans="1:4">
+      <c r="A3905"/>
+    </row>
+    <row r="3906" spans="1:4">
+      <c r="A3906"/>
+    </row>
+    <row r="3907" spans="1:4">
+      <c r="A3907"/>
+    </row>
+    <row r="3908" spans="1:4">
+      <c r="A3908"/>
+    </row>
+    <row r="3909" spans="1:4">
+      <c r="A3909"/>
+    </row>
+    <row r="3910" spans="1:4">
+      <c r="A3910"/>
+    </row>
+    <row r="3911" spans="1:4">
+      <c r="A3911"/>
+    </row>
+    <row r="3912" spans="1:4">
+      <c r="A3912"/>
+    </row>
+    <row r="3913" spans="1:4">
+      <c r="A3913"/>
+    </row>
+    <row r="3914" spans="1:4">
+      <c r="A3914"/>
+    </row>
+    <row r="3915" spans="1:4">
+      <c r="A3915"/>
+    </row>
+    <row r="3916" spans="1:4">
+      <c r="A3916"/>
+    </row>
+    <row r="3917" spans="1:4">
+      <c r="A3917"/>
+    </row>
+    <row r="3918" spans="1:4">
+      <c r="A3918"/>
+    </row>
+    <row r="3919" spans="1:4">
+      <c r="A3919"/>
+    </row>
+    <row r="3920" spans="1:4">
+      <c r="A3920"/>
+    </row>
+    <row r="3921" spans="1:4">
+      <c r="A3921"/>
+    </row>
+    <row r="3922" spans="1:4">
+      <c r="A3922"/>
+    </row>
+    <row r="3923" spans="1:4">
+      <c r="A3923"/>
+    </row>
+    <row r="3924" spans="1:4">
+      <c r="A3924"/>
+    </row>
+    <row r="3925" spans="1:4">
+      <c r="A3925"/>
+    </row>
+    <row r="3926" spans="1:4">
+      <c r="A3926"/>
+    </row>
+    <row r="3927" spans="1:4">
+      <c r="A3927"/>
+    </row>
+    <row r="3928" spans="1:4">
+      <c r="A3928"/>
+    </row>
+    <row r="3929" spans="1:4">
+      <c r="A3929"/>
+    </row>
+    <row r="3930" spans="1:4">
+      <c r="A3930"/>
+    </row>
+    <row r="3931" spans="1:4">
+      <c r="A3931"/>
+    </row>
+    <row r="3932" spans="1:4">
+      <c r="A3932"/>
+    </row>
+    <row r="3933" spans="1:4">
+      <c r="A3933"/>
+    </row>
+    <row r="3934" spans="1:4">
+      <c r="A3934"/>
+    </row>
+    <row r="3935" spans="1:4">
+      <c r="A3935"/>
+    </row>
+    <row r="3936" spans="1:4">
+      <c r="A3936"/>
+    </row>
+    <row r="3937" spans="1:4">
+      <c r="A3937"/>
+    </row>
+    <row r="3938" spans="1:4">
+      <c r="A3938"/>
+    </row>
+    <row r="3939" spans="1:4">
+      <c r="A3939"/>
+    </row>
+    <row r="3940" spans="1:4">
+      <c r="A3940"/>
+    </row>
+    <row r="3941" spans="1:4">
+      <c r="A3941"/>
+    </row>
+    <row r="3942" spans="1:4">
+      <c r="A3942"/>
+    </row>
+    <row r="3943" spans="1:4">
+      <c r="A3943"/>
+    </row>
+    <row r="3944" spans="1:4">
+      <c r="A3944"/>
+    </row>
+    <row r="3945" spans="1:4">
+      <c r="A3945"/>
+    </row>
+    <row r="3946" spans="1:4">
+      <c r="A3946"/>
+    </row>
+    <row r="3947" spans="1:4">
+      <c r="A3947"/>
+    </row>
+    <row r="3948" spans="1:4">
+      <c r="A3948"/>
+    </row>
+    <row r="3949" spans="1:4">
+      <c r="A3949"/>
+    </row>
+    <row r="3950" spans="1:4">
+      <c r="A3950"/>
+    </row>
+    <row r="3951" spans="1:4">
+      <c r="A3951"/>
+    </row>
+    <row r="3952" spans="1:4">
+      <c r="A3952"/>
+    </row>
+    <row r="3953" spans="1:4">
+      <c r="A3953"/>
+    </row>
+    <row r="3954" spans="1:4">
+      <c r="A3954"/>
+    </row>
+    <row r="3955" spans="1:4">
+      <c r="A3955"/>
+    </row>
+    <row r="3956" spans="1:4">
+      <c r="A3956"/>
+    </row>
+    <row r="3957" spans="1:4">
+      <c r="A3957"/>
+    </row>
+    <row r="3958" spans="1:4">
+      <c r="A3958"/>
+    </row>
+    <row r="3959" spans="1:4">
+      <c r="A3959"/>
+    </row>
+    <row r="3960" spans="1:4">
+      <c r="A3960"/>
+    </row>
+    <row r="3961" spans="1:4">
+      <c r="A3961"/>
+    </row>
+    <row r="3962" spans="1:4">
+      <c r="A3962"/>
+    </row>
+    <row r="3963" spans="1:4">
+      <c r="A3963"/>
+    </row>
+    <row r="3964" spans="1:4">
+      <c r="A3964"/>
+    </row>
+    <row r="3965" spans="1:4">
+      <c r="A3965"/>
+    </row>
+    <row r="3966" spans="1:4">
+      <c r="A3966"/>
+    </row>
+    <row r="3967" spans="1:4">
+      <c r="A3967"/>
+    </row>
+    <row r="3968" spans="1:4">
+      <c r="A3968"/>
+    </row>
+    <row r="3969" spans="1:4">
+      <c r="A3969"/>
+    </row>
+    <row r="3970" spans="1:4">
+      <c r="A3970"/>
+    </row>
+    <row r="3971" spans="1:4">
+      <c r="A3971"/>
+    </row>
+    <row r="3972" spans="1:4">
+      <c r="A3972"/>
+    </row>
+    <row r="3973" spans="1:4">
+      <c r="A3973"/>
+    </row>
+    <row r="3974" spans="1:4">
+      <c r="A3974"/>
+    </row>
+    <row r="3975" spans="1:4">
+      <c r="A3975"/>
+    </row>
+    <row r="3976" spans="1:4">
+      <c r="A3976"/>
+    </row>
+    <row r="3977" spans="1:4">
+      <c r="A3977"/>
+    </row>
+    <row r="3978" spans="1:4">
+      <c r="A3978"/>
+    </row>
+    <row r="3979" spans="1:4">
+      <c r="A3979"/>
+    </row>
+    <row r="3980" spans="1:4">
+      <c r="A3980"/>
+    </row>
+    <row r="3981" spans="1:4">
+      <c r="A3981"/>
+    </row>
+    <row r="3982" spans="1:4">
+      <c r="A3982"/>
+    </row>
+    <row r="3983" spans="1:4">
+      <c r="A3983"/>
+    </row>
+    <row r="3984" spans="1:4">
+      <c r="A3984"/>
+    </row>
+    <row r="3985" spans="1:4">
+      <c r="A3985"/>
+    </row>
+    <row r="3986" spans="1:4">
+      <c r="A3986"/>
+    </row>
+    <row r="3987" spans="1:4">
+      <c r="A3987"/>
+    </row>
+    <row r="3988" spans="1:4">
+      <c r="A3988"/>
+    </row>
+    <row r="3989" spans="1:4">
+      <c r="A3989"/>
+    </row>
+    <row r="3990" spans="1:4">
+      <c r="A3990"/>
+    </row>
+    <row r="3991" spans="1:4">
+      <c r="A3991"/>
+    </row>
+    <row r="3992" spans="1:4">
+      <c r="A3992"/>
+    </row>
+    <row r="3993" spans="1:4">
+      <c r="A3993"/>
+    </row>
+    <row r="3994" spans="1:4">
+      <c r="A3994"/>
+    </row>
+    <row r="3995" spans="1:4">
+      <c r="A3995"/>
+    </row>
+    <row r="3996" spans="1:4">
+      <c r="A3996"/>
+    </row>
+    <row r="3997" spans="1:4">
+      <c r="A3997"/>
+    </row>
+    <row r="3998" spans="1:4">
+      <c r="A3998"/>
+    </row>
+    <row r="3999" spans="1:4">
+      <c r="A3999"/>
+    </row>
+    <row r="4000" spans="1:4">
+      <c r="A4000"/>
+    </row>
+    <row r="4001" spans="1:4">
+      <c r="A4001"/>
+    </row>
+    <row r="4002" spans="1:4">
+      <c r="A4002"/>
+    </row>
+    <row r="4003" spans="1:4">
+      <c r="A4003"/>
+    </row>
+    <row r="4004" spans="1:4">
+      <c r="A4004"/>
+    </row>
+    <row r="4005" spans="1:4">
+      <c r="A4005"/>
+    </row>
+    <row r="4006" spans="1:4">
+      <c r="A4006"/>
+    </row>
+    <row r="4007" spans="1:4">
+      <c r="A4007"/>
+    </row>
+    <row r="4008" spans="1:4">
+      <c r="A4008"/>
+    </row>
+    <row r="4009" spans="1:4">
+      <c r="A4009"/>
+    </row>
+    <row r="4010" spans="1:4">
+      <c r="A4010"/>
+    </row>
+    <row r="4011" spans="1:4">
+      <c r="A4011"/>
+    </row>
+    <row r="4012" spans="1:4">
+      <c r="A4012"/>
+    </row>
+    <row r="4013" spans="1:4">
+      <c r="A4013"/>
+    </row>
+    <row r="4014" spans="1:4">
+      <c r="A4014"/>
+    </row>
+    <row r="4015" spans="1:4">
+      <c r="A4015"/>
+    </row>
+    <row r="4016" spans="1:4">
+      <c r="A4016"/>
+    </row>
+    <row r="4017" spans="1:4">
+      <c r="A4017"/>
+    </row>
+    <row r="4018" spans="1:4">
+      <c r="A4018"/>
+    </row>
+    <row r="4019" spans="1:4">
+      <c r="A4019"/>
+    </row>
+    <row r="4020" spans="1:4">
+      <c r="A4020"/>
+    </row>
+    <row r="4021" spans="1:4">
+      <c r="A4021"/>
+    </row>
+    <row r="4022" spans="1:4">
+      <c r="A4022"/>
+    </row>
+    <row r="4023" spans="1:4">
+      <c r="A4023"/>
+    </row>
+    <row r="4024" spans="1:4">
+      <c r="A4024"/>
+    </row>
+    <row r="4025" spans="1:4">
+      <c r="A4025"/>
+    </row>
+    <row r="4026" spans="1:4">
+      <c r="A4026"/>
+    </row>
+    <row r="4027" spans="1:4">
+      <c r="A4027"/>
+    </row>
+    <row r="4028" spans="1:4">
+      <c r="A4028"/>
+    </row>
+    <row r="4029" spans="1:4">
+      <c r="A4029"/>
+    </row>
+    <row r="4030" spans="1:4">
+      <c r="A4030"/>
+    </row>
+    <row r="4031" spans="1:4">
+      <c r="A4031"/>
+    </row>
+    <row r="4032" spans="1:4">
+      <c r="A4032"/>
+    </row>
+    <row r="4033" spans="1:4">
+      <c r="A4033"/>
+    </row>
+    <row r="4034" spans="1:4">
+      <c r="A4034"/>
+    </row>
+    <row r="4035" spans="1:4">
+      <c r="A4035"/>
+    </row>
+    <row r="4036" spans="1:4">
+      <c r="A4036"/>
+    </row>
+    <row r="4037" spans="1:4">
+      <c r="A4037"/>
+    </row>
+    <row r="4038" spans="1:4">
+      <c r="A4038"/>
+    </row>
+    <row r="4039" spans="1:4">
+      <c r="A4039"/>
+    </row>
+    <row r="4040" spans="1:4">
+      <c r="A4040"/>
+    </row>
+    <row r="4041" spans="1:4">
+      <c r="A4041"/>
+    </row>
+    <row r="4042" spans="1:4">
+      <c r="A4042"/>
+    </row>
+    <row r="4043" spans="1:4">
+      <c r="A4043"/>
+    </row>
+    <row r="4044" spans="1:4">
+      <c r="A4044"/>
+    </row>
+    <row r="4045" spans="1:4">
+      <c r="A4045"/>
+    </row>
+    <row r="4046" spans="1:4">
+      <c r="A4046"/>
+    </row>
+    <row r="4047" spans="1:4">
+      <c r="A4047"/>
+    </row>
+    <row r="4048" spans="1:4">
+      <c r="A4048"/>
+    </row>
+    <row r="4049" spans="1:4">
+      <c r="A4049"/>
+    </row>
+    <row r="4050" spans="1:4">
+      <c r="A4050"/>
+    </row>
+    <row r="4051" spans="1:4">
+      <c r="A4051"/>
+    </row>
+    <row r="4052" spans="1:4">
+      <c r="A4052"/>
+    </row>
+    <row r="4053" spans="1:4">
+      <c r="A4053"/>
+    </row>
+    <row r="4054" spans="1:4">
+      <c r="A4054"/>
+    </row>
+    <row r="4055" spans="1:4">
+      <c r="A4055"/>
+    </row>
+    <row r="4056" spans="1:4">
+      <c r="A4056"/>
+    </row>
+    <row r="4057" spans="1:4">
+      <c r="A4057"/>
+    </row>
+    <row r="4058" spans="1:4">
+      <c r="A4058"/>
+    </row>
+    <row r="4059" spans="1:4">
+      <c r="A4059"/>
+    </row>
+    <row r="4060" spans="1:4">
+      <c r="A4060"/>
+    </row>
+    <row r="4061" spans="1:4">
+      <c r="A4061"/>
+    </row>
+    <row r="4062" spans="1:4">
+      <c r="A4062"/>
+    </row>
+    <row r="4063" spans="1:4">
+      <c r="A4063"/>
+    </row>
+    <row r="4064" spans="1:4">
+      <c r="A4064"/>
+    </row>
+    <row r="4065" spans="1:4">
+      <c r="A4065"/>
+    </row>
+    <row r="4066" spans="1:4">
+      <c r="A4066"/>
+    </row>
+    <row r="4067" spans="1:4">
+      <c r="A4067"/>
+    </row>
+    <row r="4068" spans="1:4">
+      <c r="A4068"/>
+    </row>
+    <row r="4069" spans="1:4">
+      <c r="A4069"/>
+    </row>
+    <row r="4070" spans="1:4">
+      <c r="A4070"/>
+    </row>
+    <row r="4071" spans="1:4">
+      <c r="A4071"/>
+    </row>
+    <row r="4072" spans="1:4">
+      <c r="A4072"/>
+    </row>
+    <row r="4073" spans="1:4">
+      <c r="A4073"/>
+    </row>
+    <row r="4074" spans="1:4">
+      <c r="A4074"/>
+    </row>
+    <row r="4075" spans="1:4">
+      <c r="A4075"/>
+    </row>
+    <row r="4076" spans="1:4">
+      <c r="A4076"/>
+    </row>
+    <row r="4077" spans="1:4">
+      <c r="A4077"/>
+    </row>
+    <row r="4078" spans="1:4">
+      <c r="A4078"/>
+    </row>
+    <row r="4079" spans="1:4">
+      <c r="A4079"/>
+    </row>
+    <row r="4080" spans="1:4">
+      <c r="A4080"/>
+    </row>
+    <row r="4081" spans="1:4">
+      <c r="A4081"/>
+    </row>
+    <row r="4082" spans="1:4">
+      <c r="A4082"/>
+    </row>
+    <row r="4083" spans="1:4">
+      <c r="A4083"/>
+    </row>
+    <row r="4084" spans="1:4">
+      <c r="A4084"/>
+    </row>
+    <row r="4085" spans="1:4">
+      <c r="A4085"/>
+    </row>
+    <row r="4086" spans="1:4">
+      <c r="A4086"/>
+    </row>
+    <row r="4087" spans="1:4">
+      <c r="A4087"/>
+    </row>
+    <row r="4088" spans="1:4">
+      <c r="A4088"/>
+    </row>
+    <row r="4089" spans="1:4">
+      <c r="A4089"/>
+    </row>
+    <row r="4090" spans="1:4">
+      <c r="A4090"/>
+    </row>
+    <row r="4091" spans="1:4">
+      <c r="A4091"/>
+    </row>
+    <row r="4092" spans="1:4">
+      <c r="A4092"/>
+    </row>
+    <row r="4093" spans="1:4">
+      <c r="A4093"/>
+    </row>
+    <row r="4094" spans="1:4">
+      <c r="A4094"/>
+    </row>
+    <row r="4095" spans="1:4">
+      <c r="A4095"/>
+    </row>
+    <row r="4096" spans="1:4">
+      <c r="A4096"/>
+    </row>
+    <row r="4097" spans="1:4">
+      <c r="A4097"/>
+    </row>
+    <row r="4098" spans="1:4">
+      <c r="A4098"/>
+    </row>
+    <row r="4099" spans="1:4">
+      <c r="A4099"/>
+    </row>
+    <row r="4100" spans="1:4">
+      <c r="A4100"/>
+    </row>
+    <row r="4101" spans="1:4">
+      <c r="A4101"/>
+    </row>
+    <row r="4102" spans="1:4">
+      <c r="A4102"/>
+    </row>
+    <row r="4103" spans="1:4">
+      <c r="A4103"/>
+    </row>
+    <row r="4104" spans="1:4">
+      <c r="A4104"/>
+    </row>
+    <row r="4105" spans="1:4">
+      <c r="A4105"/>
+    </row>
+    <row r="4106" spans="1:4">
+      <c r="A4106"/>
+    </row>
+    <row r="4107" spans="1:4">
+      <c r="A4107"/>
+    </row>
+    <row r="4108" spans="1:4">
+      <c r="A4108"/>
+    </row>
+    <row r="4109" spans="1:4">
+      <c r="A4109"/>
+    </row>
+    <row r="4110" spans="1:4">
+      <c r="A4110"/>
+    </row>
+    <row r="4111" spans="1:4">
+      <c r="A4111"/>
+    </row>
+    <row r="4112" spans="1:4">
+      <c r="A4112"/>
+    </row>
+    <row r="4113" spans="1:4">
+      <c r="A4113"/>
+    </row>
+    <row r="4114" spans="1:4">
+      <c r="A4114"/>
+    </row>
+    <row r="4115" spans="1:4">
+      <c r="A4115"/>
+    </row>
+    <row r="4116" spans="1:4">
+      <c r="A4116"/>
+    </row>
+    <row r="4117" spans="1:4">
+      <c r="A4117"/>
+    </row>
+    <row r="4118" spans="1:4">
+      <c r="A4118"/>
+    </row>
+    <row r="4119" spans="1:4">
+      <c r="A4119"/>
+    </row>
+    <row r="4120" spans="1:4">
+      <c r="A4120"/>
+    </row>
+    <row r="4121" spans="1:4">
+      <c r="A4121"/>
+    </row>
+    <row r="4122" spans="1:4">
+      <c r="A4122"/>
+    </row>
+    <row r="4123" spans="1:4">
+      <c r="A4123"/>
+    </row>
+    <row r="4124" spans="1:4">
+      <c r="A4124"/>
+    </row>
+    <row r="4125" spans="1:4">
+      <c r="A4125"/>
+    </row>
+    <row r="4126" spans="1:4">
+      <c r="A4126"/>
+    </row>
+    <row r="4127" spans="1:4">
+      <c r="A4127"/>
+    </row>
+    <row r="4128" spans="1:4">
+      <c r="A4128"/>
+    </row>
+    <row r="4129" spans="1:4">
+      <c r="A4129"/>
+    </row>
+    <row r="4130" spans="1:4">
+      <c r="A4130"/>
+    </row>
+    <row r="4131" spans="1:4">
+      <c r="A4131"/>
+    </row>
+    <row r="4132" spans="1:4">
+      <c r="A4132"/>
+    </row>
+    <row r="4133" spans="1:4">
+      <c r="A4133"/>
+    </row>
+    <row r="4134" spans="1:4">
+      <c r="A4134"/>
+    </row>
+    <row r="4135" spans="1:4">
+      <c r="A4135"/>
+    </row>
+    <row r="4136" spans="1:4">
+      <c r="A4136"/>
+    </row>
+    <row r="4137" spans="1:4">
+      <c r="A4137"/>
+    </row>
+    <row r="4138" spans="1:4">
+      <c r="A4138"/>
+    </row>
+    <row r="4139" spans="1:4">
+      <c r="A4139"/>
+    </row>
+    <row r="4140" spans="1:4">
+      <c r="A4140"/>
+    </row>
+    <row r="4141" spans="1:4">
+      <c r="A4141"/>
+    </row>
+    <row r="4142" spans="1:4">
+      <c r="A4142"/>
+    </row>
+    <row r="4143" spans="1:4">
+      <c r="A4143"/>
+    </row>
+    <row r="4144" spans="1:4">
+      <c r="A4144"/>
+    </row>
+    <row r="4145" spans="1:4">
+      <c r="A4145"/>
+    </row>
+    <row r="4146" spans="1:4">
+      <c r="A4146"/>
+    </row>
+    <row r="4147" spans="1:4">
+      <c r="A4147"/>
+    </row>
+    <row r="4148" spans="1:4">
+      <c r="A4148"/>
+    </row>
+    <row r="4149" spans="1:4">
+      <c r="A4149"/>
+    </row>
+    <row r="4150" spans="1:4">
+      <c r="A4150"/>
+    </row>
+    <row r="4151" spans="1:4">
+      <c r="A4151"/>
+    </row>
+    <row r="4152" spans="1:4">
+      <c r="A4152"/>
+    </row>
+    <row r="4153" spans="1:4">
+      <c r="A4153"/>
+    </row>
+    <row r="4154" spans="1:4">
+      <c r="A4154"/>
+    </row>
+    <row r="4155" spans="1:4">
+      <c r="A4155"/>
+    </row>
+    <row r="4156" spans="1:4">
+      <c r="A4156"/>
+    </row>
+    <row r="4157" spans="1:4">
+      <c r="A4157"/>
+    </row>
+    <row r="4158" spans="1:4">
+      <c r="A4158"/>
+    </row>
+    <row r="4159" spans="1:4">
+      <c r="A4159"/>
+    </row>
+    <row r="4160" spans="1:4">
+      <c r="A4160"/>
+    </row>
+    <row r="4161" spans="1:4">
+      <c r="A4161"/>
+    </row>
+    <row r="4162" spans="1:4">
+      <c r="A4162"/>
+    </row>
+    <row r="4163" spans="1:4">
+      <c r="A4163"/>
+    </row>
+    <row r="4164" spans="1:4">
+      <c r="A4164"/>
+    </row>
+    <row r="4165" spans="1:4">
+      <c r="A4165"/>
+    </row>
+    <row r="4166" spans="1:4">
+      <c r="A4166"/>
+    </row>
+    <row r="4167" spans="1:4">
+      <c r="A4167"/>
+    </row>
+    <row r="4168" spans="1:4">
+      <c r="A4168"/>
+    </row>
+    <row r="4169" spans="1:4">
+      <c r="A4169"/>
+    </row>
+    <row r="4170" spans="1:4">
+      <c r="A4170"/>
+    </row>
+    <row r="4171" spans="1:4">
+      <c r="A4171"/>
+    </row>
+    <row r="4172" spans="1:4">
+      <c r="A4172"/>
+    </row>
+    <row r="4173" spans="1:4">
+      <c r="A4173"/>
+    </row>
+    <row r="4174" spans="1:4">
+      <c r="A4174"/>
+    </row>
+    <row r="4175" spans="1:4">
+      <c r="A4175"/>
+    </row>
+    <row r="4176" spans="1:4">
+      <c r="A4176"/>
+    </row>
+    <row r="4177" spans="1:4">
+      <c r="A4177"/>
+    </row>
+    <row r="4178" spans="1:4">
+      <c r="A4178"/>
+    </row>
+    <row r="4179" spans="1:4">
+      <c r="A4179"/>
+    </row>
+    <row r="4180" spans="1:4">
+      <c r="A4180"/>
+    </row>
+    <row r="4181" spans="1:4">
+      <c r="A4181"/>
+    </row>
+    <row r="4182" spans="1:4">
+      <c r="A4182"/>
+    </row>
+    <row r="4183" spans="1:4">
+      <c r="A4183"/>
+    </row>
+    <row r="4184" spans="1:4">
+      <c r="A4184"/>
+    </row>
+    <row r="4185" spans="1:4">
+      <c r="A4185"/>
+    </row>
+    <row r="4186" spans="1:4">
+      <c r="A4186"/>
+    </row>
+    <row r="4187" spans="1:4">
+      <c r="A4187"/>
+    </row>
+    <row r="4188" spans="1:4">
+      <c r="A4188"/>
+    </row>
+    <row r="4189" spans="1:4">
+      <c r="A4189"/>
+    </row>
+    <row r="4190" spans="1:4">
+      <c r="A4190"/>
+    </row>
+    <row r="4191" spans="1:4">
+      <c r="A4191"/>
+    </row>
+    <row r="4192" spans="1:4">
+      <c r="A4192"/>
+    </row>
+    <row r="4193" spans="1:4">
+      <c r="A4193"/>
+    </row>
+    <row r="4194" spans="1:4">
+      <c r="A4194"/>
+    </row>
+    <row r="4195" spans="1:4">
+      <c r="A4195"/>
+    </row>
+    <row r="4196" spans="1:4">
+      <c r="A4196"/>
+    </row>
+    <row r="4197" spans="1:4">
+      <c r="A4197"/>
+    </row>
+    <row r="4198" spans="1:4">
+      <c r="A4198"/>
+    </row>
+    <row r="4199" spans="1:4">
+      <c r="A4199"/>
+    </row>
+    <row r="4200" spans="1:4">
+      <c r="A4200"/>
+    </row>
+    <row r="4201" spans="1:4">
+      <c r="A4201"/>
+    </row>
+    <row r="4202" spans="1:4">
+      <c r="A4202"/>
+    </row>
+    <row r="4203" spans="1:4">
+      <c r="A4203"/>
+    </row>
+    <row r="4204" spans="1:4">
+      <c r="A4204"/>
+    </row>
+    <row r="4205" spans="1:4">
+      <c r="A4205"/>
+    </row>
+    <row r="4206" spans="1:4">
+      <c r="A4206"/>
+    </row>
+    <row r="4207" spans="1:4">
+      <c r="A4207"/>
+    </row>
+    <row r="4208" spans="1:4">
+      <c r="A4208"/>
+    </row>
+    <row r="4209" spans="1:4">
+      <c r="A4209"/>
+    </row>
+    <row r="4210" spans="1:4">
+      <c r="A4210"/>
+    </row>
+    <row r="4211" spans="1:4">
+      <c r="A4211"/>
+    </row>
+    <row r="4212" spans="1:4">
+      <c r="A4212"/>
+    </row>
+    <row r="4213" spans="1:4">
+      <c r="A4213"/>
+    </row>
+    <row r="4214" spans="1:4">
+      <c r="A4214"/>
+    </row>
+    <row r="4215" spans="1:4">
+      <c r="A4215"/>
+    </row>
+    <row r="4216" spans="1:4">
+      <c r="A4216"/>
+    </row>
+    <row r="4217" spans="1:4">
+      <c r="A4217"/>
+    </row>
+    <row r="4218" spans="1:4">
+      <c r="A4218"/>
+    </row>
+    <row r="4219" spans="1:4">
+      <c r="A4219"/>
+    </row>
+    <row r="4220" spans="1:4">
+      <c r="A4220"/>
+    </row>
+    <row r="4221" spans="1:4">
+      <c r="A4221"/>
+    </row>
+    <row r="4222" spans="1:4">
+      <c r="A4222"/>
+    </row>
+    <row r="4223" spans="1:4">
+      <c r="A4223"/>
+    </row>
+    <row r="4224" spans="1:4">
+      <c r="A4224"/>
+    </row>
+    <row r="4225" spans="1:4">
+      <c r="A4225"/>
+    </row>
+    <row r="4226" spans="1:4">
+      <c r="A4226"/>
+    </row>
+    <row r="4227" spans="1:4">
+      <c r="A4227"/>
+    </row>
+    <row r="4228" spans="1:4">
+      <c r="A4228"/>
+    </row>
+    <row r="4229" spans="1:4">
+      <c r="A4229"/>
+    </row>
+    <row r="4230" spans="1:4">
+      <c r="A4230"/>
+    </row>
+    <row r="4231" spans="1:4">
+      <c r="A4231"/>
+    </row>
+    <row r="4232" spans="1:4">
+      <c r="A4232"/>
+    </row>
+    <row r="4233" spans="1:4">
+      <c r="A4233"/>
+    </row>
+    <row r="4234" spans="1:4">
+      <c r="A4234"/>
+    </row>
+    <row r="4235" spans="1:4">
+      <c r="A4235"/>
+    </row>
+    <row r="4236" spans="1:4">
+      <c r="A4236"/>
+    </row>
+    <row r="4237" spans="1:4">
+      <c r="A4237"/>
+    </row>
+    <row r="4238" spans="1:4">
+      <c r="A4238"/>
+    </row>
+    <row r="4239" spans="1:4">
+      <c r="A4239"/>
+    </row>
+    <row r="4240" spans="1:4">
+      <c r="A4240"/>
+    </row>
+    <row r="4241" spans="1:4">
+      <c r="A4241"/>
+    </row>
+    <row r="4242" spans="1:4">
+      <c r="A4242"/>
+    </row>
+    <row r="4243" spans="1:4">
+      <c r="A4243"/>
+    </row>
+    <row r="4244" spans="1:4">
+      <c r="A4244"/>
+    </row>
+    <row r="4245" spans="1:4">
+      <c r="A4245"/>
+    </row>
+    <row r="4246" spans="1:4">
+      <c r="A4246"/>
+    </row>
+    <row r="4247" spans="1:4">
+      <c r="A4247"/>
+    </row>
+    <row r="4248" spans="1:4">
+      <c r="A4248"/>
+    </row>
+    <row r="4249" spans="1:4">
+      <c r="A4249"/>
+    </row>
+    <row r="4250" spans="1:4">
+      <c r="A4250"/>
+    </row>
+    <row r="4251" spans="1:4">
+      <c r="A4251"/>
+    </row>
+    <row r="4252" spans="1:4">
+      <c r="A4252"/>
+    </row>
+    <row r="4253" spans="1:4">
+      <c r="A4253"/>
+    </row>
+    <row r="4254" spans="1:4">
+      <c r="A4254"/>
+    </row>
+    <row r="4255" spans="1:4">
+      <c r="A4255"/>
+    </row>
+    <row r="4256" spans="1:4">
+      <c r="A4256"/>
+    </row>
+    <row r="4257" spans="1:4">
+      <c r="A4257"/>
+    </row>
+    <row r="4258" spans="1:4">
+      <c r="A4258"/>
+    </row>
+    <row r="4259" spans="1:4">
+      <c r="A4259"/>
+    </row>
+    <row r="4260" spans="1:4">
+      <c r="A4260"/>
+    </row>
+    <row r="4261" spans="1:4">
+      <c r="A4261"/>
+    </row>
+    <row r="4262" spans="1:4">
+      <c r="A4262"/>
+    </row>
+    <row r="4263" spans="1:4">
+      <c r="A4263"/>
+    </row>
+    <row r="4264" spans="1:4">
+      <c r="A4264"/>
+    </row>
+    <row r="4265" spans="1:4">
+      <c r="A4265"/>
+    </row>
+    <row r="4266" spans="1:4">
+      <c r="A4266"/>
+    </row>
+    <row r="4267" spans="1:4">
+      <c r="A4267"/>
+    </row>
+    <row r="4268" spans="1:4">
+      <c r="A4268"/>
+    </row>
+    <row r="4269" spans="1:4">
+      <c r="A4269"/>
+    </row>
+    <row r="4270" spans="1:4">
+      <c r="A4270"/>
+    </row>
+    <row r="4271" spans="1:4">
+      <c r="A4271"/>
+    </row>
+    <row r="4272" spans="1:4">
+      <c r="A4272"/>
+    </row>
+    <row r="4273" spans="1:4">
+      <c r="A4273"/>
+    </row>
+    <row r="4274" spans="1:4">
+      <c r="A4274"/>
+    </row>
+    <row r="4275" spans="1:4">
+      <c r="A4275"/>
+    </row>
+    <row r="4276" spans="1:4">
+      <c r="A4276"/>
+    </row>
+    <row r="4277" spans="1:4">
+      <c r="A4277"/>
+    </row>
+    <row r="4278" spans="1:4">
+      <c r="A4278"/>
+    </row>
+    <row r="4279" spans="1:4">
+      <c r="A4279"/>
+    </row>
+    <row r="4280" spans="1:4">
+      <c r="A4280"/>
+    </row>
+    <row r="4281" spans="1:4">
+      <c r="A4281"/>
+    </row>
+    <row r="4282" spans="1:4">
+      <c r="A4282"/>
+    </row>
+    <row r="4283" spans="1:4">
+      <c r="A4283"/>
+    </row>
+    <row r="4284" spans="1:4">
+      <c r="A4284"/>
+    </row>
+    <row r="4285" spans="1:4">
+      <c r="A4285"/>
+    </row>
+    <row r="4286" spans="1:4">
+      <c r="A4286"/>
+    </row>
+    <row r="4287" spans="1:4">
+      <c r="A4287"/>
+    </row>
+    <row r="4288" spans="1:4">
+      <c r="A4288"/>
+    </row>
+    <row r="4289" spans="1:4">
+      <c r="A4289"/>
+    </row>
+    <row r="4290" spans="1:4">
+      <c r="A4290"/>
+    </row>
+    <row r="4291" spans="1:4">
+      <c r="A4291"/>
+    </row>
+    <row r="4292" spans="1:4">
+      <c r="A4292"/>
+    </row>
+    <row r="4293" spans="1:4">
+      <c r="A4293"/>
+    </row>
+    <row r="4294" spans="1:4">
+      <c r="A4294"/>
+    </row>
+    <row r="4295" spans="1:4">
+      <c r="A4295"/>
+    </row>
+    <row r="4296" spans="1:4">
+      <c r="A4296"/>
+    </row>
+    <row r="4297" spans="1:4">
+      <c r="A4297"/>
+    </row>
+    <row r="4298" spans="1:4">
+      <c r="A4298"/>
+    </row>
+    <row r="4299" spans="1:4">
+      <c r="A4299"/>
+    </row>
+    <row r="4300" spans="1:4">
+      <c r="A4300"/>
+    </row>
+    <row r="4301" spans="1:4">
+      <c r="A4301"/>
+    </row>
+    <row r="4302" spans="1:4">
+      <c r="A4302"/>
+    </row>
+    <row r="4303" spans="1:4">
+      <c r="A4303"/>
+    </row>
+    <row r="4304" spans="1:4">
+      <c r="A4304"/>
+    </row>
+    <row r="4305" spans="1:4">
+      <c r="A4305"/>
+    </row>
+    <row r="4306" spans="1:4">
+      <c r="A4306"/>
+    </row>
+    <row r="4307" spans="1:4">
+      <c r="A4307"/>
+    </row>
+    <row r="4308" spans="1:4">
+      <c r="A4308"/>
+    </row>
+    <row r="4309" spans="1:4">
+      <c r="A4309"/>
+    </row>
+    <row r="4310" spans="1:4">
+      <c r="A4310"/>
+    </row>
+    <row r="4311" spans="1:4">
+      <c r="A4311"/>
+    </row>
+    <row r="4312" spans="1:4">
+      <c r="A4312"/>
+    </row>
+    <row r="4313" spans="1:4">
+      <c r="A4313"/>
+    </row>
+    <row r="4314" spans="1:4">
+      <c r="A4314"/>
+    </row>
+    <row r="4315" spans="1:4">
+      <c r="A4315"/>
+    </row>
+    <row r="4316" spans="1:4">
+      <c r="A4316"/>
+    </row>
+    <row r="4317" spans="1:4">
+      <c r="A4317"/>
+    </row>
+    <row r="4318" spans="1:4">
+      <c r="A4318"/>
+    </row>
+    <row r="4319" spans="1:4">
+      <c r="A4319"/>
+    </row>
+    <row r="4320" spans="1:4">
+      <c r="A4320"/>
+    </row>
+    <row r="4321" spans="1:4">
+      <c r="A4321"/>
+    </row>
+    <row r="4322" spans="1:4">
+      <c r="A4322"/>
+    </row>
+    <row r="4323" spans="1:4">
+      <c r="A4323"/>
+    </row>
+    <row r="4324" spans="1:4">
+      <c r="A4324"/>
+    </row>
+    <row r="4325" spans="1:4">
+      <c r="A4325"/>
+    </row>
+    <row r="4326" spans="1:4">
+      <c r="A4326"/>
+    </row>
+    <row r="4327" spans="1:4">
+      <c r="A4327"/>
+    </row>
+    <row r="4328" spans="1:4">
+      <c r="A4328"/>
+    </row>
+    <row r="4329" spans="1:4">
+      <c r="A4329"/>
+    </row>
+    <row r="4330" spans="1:4">
+      <c r="A4330"/>
+    </row>
+    <row r="4331" spans="1:4">
+      <c r="A4331"/>
+    </row>
+    <row r="4332" spans="1:4">
+      <c r="A4332"/>
+    </row>
+    <row r="4333" spans="1:4">
+      <c r="A4333"/>
+    </row>
+    <row r="4334" spans="1:4">
+      <c r="A4334"/>
+    </row>
+    <row r="4335" spans="1:4">
+      <c r="A4335"/>
+    </row>
+    <row r="4336" spans="1:4">
+      <c r="A4336"/>
+    </row>
+    <row r="4337" spans="1:4">
+      <c r="A4337"/>
+    </row>
+    <row r="4338" spans="1:4">
+      <c r="A4338"/>
+    </row>
+    <row r="4339" spans="1:4">
+      <c r="A4339"/>
+    </row>
+    <row r="4340" spans="1:4">
+      <c r="A4340"/>
+    </row>
+    <row r="4341" spans="1:4">
+      <c r="A4341"/>
+    </row>
+    <row r="4342" spans="1:4">
+      <c r="A4342"/>
+    </row>
+    <row r="4343" spans="1:4">
+      <c r="A4343"/>
+    </row>
+    <row r="4344" spans="1:4">
+      <c r="A4344"/>
+    </row>
+    <row r="4345" spans="1:4">
+      <c r="A4345"/>
+    </row>
+    <row r="4346" spans="1:4">
+      <c r="A4346"/>
+    </row>
+    <row r="4347" spans="1:4">
+      <c r="A4347"/>
+    </row>
+    <row r="4348" spans="1:4">
+      <c r="A4348"/>
+    </row>
+    <row r="4349" spans="1:4">
+      <c r="A4349"/>
+    </row>
+    <row r="4350" spans="1:4">
+      <c r="A4350"/>
+    </row>
+    <row r="4351" spans="1:4">
+      <c r="A4351"/>
+    </row>
+    <row r="4352" spans="1:4">
+      <c r="A4352"/>
+    </row>
+    <row r="4353" spans="1:4">
+      <c r="A4353"/>
+    </row>
+    <row r="4354" spans="1:4">
+      <c r="A4354"/>
+    </row>
+    <row r="4355" spans="1:4">
+      <c r="A4355"/>
+    </row>
+    <row r="4356" spans="1:4">
+      <c r="A4356"/>
+    </row>
+    <row r="4357" spans="1:4">
+      <c r="A4357"/>
+    </row>
+    <row r="4358" spans="1:4">
+      <c r="A4358"/>
+    </row>
+    <row r="4359" spans="1:4">
+      <c r="A4359"/>
+    </row>
+    <row r="4360" spans="1:4">
+      <c r="A4360"/>
+    </row>
+    <row r="4361" spans="1:4">
+      <c r="A4361"/>
+    </row>
+    <row r="4362" spans="1:4">
+      <c r="A4362"/>
+    </row>
+    <row r="4363" spans="1:4">
+      <c r="A4363"/>
+    </row>
+    <row r="4364" spans="1:4">
+      <c r="A4364"/>
+    </row>
+    <row r="4365" spans="1:4">
+      <c r="A4365"/>
+    </row>
+    <row r="4366" spans="1:4">
+      <c r="A4366"/>
+    </row>
+    <row r="4367" spans="1:4">
+      <c r="A4367"/>
+    </row>
+    <row r="4368" spans="1:4">
+      <c r="A4368"/>
+    </row>
+    <row r="4369" spans="1:4">
+      <c r="A4369"/>
+    </row>
+    <row r="4370" spans="1:4">
+      <c r="A4370"/>
+    </row>
+    <row r="4371" spans="1:4">
+      <c r="A4371"/>
+    </row>
+    <row r="4372" spans="1:4">
+      <c r="A4372"/>
+    </row>
+    <row r="4373" spans="1:4">
+      <c r="A4373"/>
+    </row>
+    <row r="4374" spans="1:4">
+      <c r="A4374"/>
+    </row>
+    <row r="4375" spans="1:4">
+      <c r="A4375"/>
+    </row>
+    <row r="4376" spans="1:4">
+      <c r="A4376"/>
+    </row>
+    <row r="4377" spans="1:4">
+      <c r="A4377"/>
+    </row>
+    <row r="4378" spans="1:4">
+      <c r="A4378"/>
+    </row>
+    <row r="4379" spans="1:4">
+      <c r="A4379"/>
+    </row>
+    <row r="4380" spans="1:4">
+      <c r="A4380"/>
+    </row>
+    <row r="4381" spans="1:4">
+      <c r="A4381"/>
+    </row>
+    <row r="4382" spans="1:4">
+      <c r="A4382"/>
+    </row>
+    <row r="4383" spans="1:4">
+      <c r="A4383"/>
+    </row>
+    <row r="4384" spans="1:4">
+      <c r="A4384"/>
+    </row>
+    <row r="4385" spans="1:4">
+      <c r="A4385"/>
+    </row>
+    <row r="4386" spans="1:4">
+      <c r="A4386"/>
+    </row>
+    <row r="4387" spans="1:4">
+      <c r="A4387"/>
+    </row>
+    <row r="4388" spans="1:4">
+      <c r="A4388"/>
+    </row>
+    <row r="4389" spans="1:4">
+      <c r="A4389"/>
+    </row>
+    <row r="4390" spans="1:4">
+      <c r="A4390"/>
+    </row>
+    <row r="4391" spans="1:4">
+      <c r="A4391"/>
+    </row>
+    <row r="4392" spans="1:4">
+      <c r="A4392"/>
+    </row>
+    <row r="4393" spans="1:4">
+      <c r="A4393"/>
+    </row>
+    <row r="4394" spans="1:4">
+      <c r="A4394"/>
+    </row>
+    <row r="4395" spans="1:4">
+      <c r="A4395"/>
+    </row>
+    <row r="4396" spans="1:4">
+      <c r="A4396"/>
+    </row>
+    <row r="4397" spans="1:4">
+      <c r="A4397"/>
+    </row>
+    <row r="4398" spans="1:4">
+      <c r="A4398"/>
+    </row>
+    <row r="4399" spans="1:4">
+      <c r="A4399"/>
+    </row>
+    <row r="4400" spans="1:4">
+      <c r="A4400"/>
+    </row>
+    <row r="4401" spans="1:4">
+      <c r="A4401"/>
+    </row>
+    <row r="4402" spans="1:4">
+      <c r="A4402"/>
+    </row>
+    <row r="4403" spans="1:4">
+      <c r="A4403"/>
+    </row>
+    <row r="4404" spans="1:4">
+      <c r="A4404"/>
+    </row>
+    <row r="4405" spans="1:4">
+      <c r="A4405"/>
+    </row>
+    <row r="4406" spans="1:4">
+      <c r="A4406"/>
+    </row>
+    <row r="4407" spans="1:4">
+      <c r="A4407"/>
+    </row>
+    <row r="4408" spans="1:4">
+      <c r="A4408"/>
+    </row>
+    <row r="4409" spans="1:4">
+      <c r="A4409"/>
+    </row>
+    <row r="4410" spans="1:4">
+      <c r="A4410"/>
+    </row>
+    <row r="4411" spans="1:4">
+      <c r="A4411"/>
+    </row>
+    <row r="4412" spans="1:4">
+      <c r="A4412"/>
+    </row>
+    <row r="4413" spans="1:4">
+      <c r="A4413"/>
+    </row>
+    <row r="4414" spans="1:4">
+      <c r="A4414"/>
+    </row>
+    <row r="4415" spans="1:4">
+      <c r="A4415"/>
+    </row>
+    <row r="4416" spans="1:4">
+      <c r="A4416"/>
+    </row>
+    <row r="4417" spans="1:4">
+      <c r="A4417"/>
+    </row>
+    <row r="4418" spans="1:4">
+      <c r="A4418"/>
+    </row>
+    <row r="4419" spans="1:4">
+      <c r="A4419"/>
+    </row>
+    <row r="4420" spans="1:4">
+      <c r="A4420"/>
+    </row>
+    <row r="4421" spans="1:4">
+      <c r="A4421"/>
+    </row>
+    <row r="4422" spans="1:4">
+      <c r="A4422"/>
+    </row>
+    <row r="4423" spans="1:4">
+      <c r="A4423"/>
+    </row>
+    <row r="4424" spans="1:4">
+      <c r="A4424"/>
+    </row>
+    <row r="4425" spans="1:4">
+      <c r="A4425"/>
+    </row>
+    <row r="4426" spans="1:4">
+      <c r="A4426"/>
+    </row>
+    <row r="4427" spans="1:4">
+      <c r="A4427"/>
+    </row>
+    <row r="4428" spans="1:4">
+      <c r="A4428"/>
+    </row>
+    <row r="4429" spans="1:4">
+      <c r="A4429"/>
+    </row>
+    <row r="4430" spans="1:4">
+      <c r="A4430"/>
+    </row>
+    <row r="4431" spans="1:4">
+      <c r="A4431"/>
+    </row>
+    <row r="4432" spans="1:4">
+      <c r="A4432"/>
+    </row>
+    <row r="4433" spans="1:4">
+      <c r="A4433"/>
+    </row>
+    <row r="4434" spans="1:4">
+      <c r="A4434"/>
+    </row>
+    <row r="4435" spans="1:4">
+      <c r="A4435"/>
+    </row>
+    <row r="4436" spans="1:4">
+      <c r="A4436"/>
+    </row>
+    <row r="4437" spans="1:4">
+      <c r="A4437"/>
+    </row>
+    <row r="4438" spans="1:4">
+      <c r="A4438"/>
+    </row>
+    <row r="4439" spans="1:4">
+      <c r="A4439"/>
+    </row>
+    <row r="4440" spans="1:4">
+      <c r="A4440"/>
+    </row>
+    <row r="4441" spans="1:4">
+      <c r="A4441"/>
+    </row>
+    <row r="4442" spans="1:4">
+      <c r="A4442"/>
+    </row>
+    <row r="4443" spans="1:4">
+      <c r="A4443"/>
+    </row>
+    <row r="4444" spans="1:4">
+      <c r="A4444"/>
+    </row>
+    <row r="4445" spans="1:4">
+      <c r="A4445"/>
+    </row>
+    <row r="4446" spans="1:4">
+      <c r="A4446"/>
+    </row>
+    <row r="4447" spans="1:4">
+      <c r="A4447"/>
+    </row>
+    <row r="4448" spans="1:4">
+      <c r="A4448"/>
+    </row>
+    <row r="4449" spans="1:4">
+      <c r="A4449"/>
+    </row>
+    <row r="4450" spans="1:4">
+      <c r="A4450"/>
+    </row>
+    <row r="4451" spans="1:4">
+      <c r="A4451"/>
+    </row>
+    <row r="4452" spans="1:4">
+      <c r="A4452"/>
+    </row>
+    <row r="4453" spans="1:4">
+      <c r="A4453"/>
+    </row>
+    <row r="4454" spans="1:4">
+      <c r="A4454"/>
+    </row>
+    <row r="4455" spans="1:4">
+      <c r="A4455"/>
+    </row>
+    <row r="4456" spans="1:4">
+      <c r="A4456"/>
+    </row>
+    <row r="4457" spans="1:4">
+      <c r="A4457"/>
+    </row>
+    <row r="4458" spans="1:4">
+      <c r="A4458"/>
+    </row>
+    <row r="4459" spans="1:4">
+      <c r="A4459"/>
+    </row>
+    <row r="4460" spans="1:4">
+      <c r="A4460"/>
+    </row>
+    <row r="4461" spans="1:4">
+      <c r="A4461"/>
+    </row>
+    <row r="4462" spans="1:4">
+      <c r="A4462"/>
+    </row>
+    <row r="4463" spans="1:4">
+      <c r="A4463"/>
+    </row>
+    <row r="4464" spans="1:4">
+      <c r="A4464"/>
+    </row>
+    <row r="4465" spans="1:4">
+      <c r="A4465"/>
+    </row>
+    <row r="4466" spans="1:4">
+      <c r="A4466"/>
+    </row>
+    <row r="4467" spans="1:4">
+      <c r="A4467"/>
+    </row>
+    <row r="4468" spans="1:4">
+      <c r="A4468"/>
+    </row>
+    <row r="4469" spans="1:4">
+      <c r="A4469"/>
+    </row>
+    <row r="4470" spans="1:4">
+      <c r="A4470"/>
+    </row>
+    <row r="4471" spans="1:4">
+      <c r="A4471"/>
+    </row>
+    <row r="4472" spans="1:4">
+      <c r="A4472"/>
+    </row>
+    <row r="4473" spans="1:4">
+      <c r="A4473"/>
+    </row>
+    <row r="4474" spans="1:4">
+      <c r="A4474"/>
+    </row>
+    <row r="4475" spans="1:4">
+      <c r="A4475"/>
+    </row>
+    <row r="4476" spans="1:4">
+      <c r="A4476"/>
+    </row>
+    <row r="4477" spans="1:4">
+      <c r="A4477"/>
+    </row>
+    <row r="4478" spans="1:4">
+      <c r="A4478"/>
+    </row>
+    <row r="4479" spans="1:4">
+      <c r="A4479"/>
+    </row>
+    <row r="4480" spans="1:4">
+      <c r="A4480"/>
+    </row>
+    <row r="4481" spans="1:4">
+      <c r="A4481"/>
+    </row>
+    <row r="4482" spans="1:4">
+      <c r="A4482"/>
+    </row>
+    <row r="4483" spans="1:4">
+      <c r="A4483"/>
+    </row>
+    <row r="4484" spans="1:4">
+      <c r="A4484"/>
+    </row>
+    <row r="4485" spans="1:4">
+      <c r="A4485"/>
+    </row>
+    <row r="4486" spans="1:4">
+      <c r="A4486"/>
+    </row>
+    <row r="4487" spans="1:4">
+      <c r="A4487"/>
+    </row>
+    <row r="4488" spans="1:4">
+      <c r="A4488"/>
+    </row>
+    <row r="4489" spans="1:4">
+      <c r="A4489"/>
+    </row>
+    <row r="4490" spans="1:4">
+      <c r="A4490"/>
+    </row>
+    <row r="4491" spans="1:4">
+      <c r="A4491"/>
+    </row>
+    <row r="4492" spans="1:4">
+      <c r="A4492"/>
+    </row>
+    <row r="4493" spans="1:4">
+      <c r="A4493"/>
+    </row>
+    <row r="4494" spans="1:4">
+      <c r="A4494"/>
+    </row>
+    <row r="4495" spans="1:4">
+      <c r="A4495"/>
+    </row>
+    <row r="4496" spans="1:4">
+      <c r="A4496"/>
+    </row>
+    <row r="4497" spans="1:4">
+      <c r="A4497"/>
+    </row>
+    <row r="4498" spans="1:4">
+      <c r="A4498"/>
+    </row>
+    <row r="4499" spans="1:4">
+      <c r="A4499"/>
+    </row>
+    <row r="4500" spans="1:4">
+      <c r="A4500"/>
+    </row>
+    <row r="4501" spans="1:4">
+      <c r="A4501"/>
+    </row>
+    <row r="4502" spans="1:4">
+      <c r="A4502"/>
+    </row>
+    <row r="4503" spans="1:4">
+      <c r="A4503"/>
+    </row>
+    <row r="4504" spans="1:4">
+      <c r="A4504"/>
+    </row>
+    <row r="4505" spans="1:4">
+      <c r="A4505"/>
+    </row>
+    <row r="4506" spans="1:4">
+      <c r="A4506"/>
+    </row>
+    <row r="4507" spans="1:4">
+      <c r="A4507"/>
+    </row>
+    <row r="4508" spans="1:4">
+      <c r="A4508"/>
+    </row>
+    <row r="4509" spans="1:4">
+      <c r="A4509"/>
+    </row>
+    <row r="4510" spans="1:4">
+      <c r="A4510"/>
+    </row>
+    <row r="4511" spans="1:4">
+      <c r="A4511"/>
+    </row>
+    <row r="4512" spans="1:4">
+      <c r="A4512"/>
+    </row>
+    <row r="4513" spans="1:4">
+      <c r="A4513"/>
+    </row>
+    <row r="4514" spans="1:4">
+      <c r="A4514"/>
+    </row>
+    <row r="4515" spans="1:4">
+      <c r="A4515"/>
+    </row>
+    <row r="4516" spans="1:4">
+      <c r="A4516"/>
+    </row>
+    <row r="4517" spans="1:4">
+      <c r="A4517"/>
+    </row>
+    <row r="4518" spans="1:4">
+      <c r="A4518"/>
+    </row>
+    <row r="4519" spans="1:4">
+      <c r="A4519"/>
+    </row>
+    <row r="4520" spans="1:4">
+      <c r="A4520"/>
+    </row>
+    <row r="4521" spans="1:4">
+      <c r="A4521"/>
+    </row>
+    <row r="4522" spans="1:4">
+      <c r="A4522"/>
+    </row>
+    <row r="4523" spans="1:4">
+      <c r="A4523"/>
+    </row>
+    <row r="4524" spans="1:4">
+      <c r="A4524"/>
+    </row>
+    <row r="4525" spans="1:4">
+      <c r="A4525"/>
+    </row>
+    <row r="4526" spans="1:4">
+      <c r="A4526"/>
+    </row>
+    <row r="4527" spans="1:4">
+      <c r="A4527"/>
+    </row>
+    <row r="4528" spans="1:4">
+      <c r="A4528"/>
+    </row>
+    <row r="4529" spans="1:4">
+      <c r="A4529"/>
+    </row>
+    <row r="4530" spans="1:4">
+      <c r="A4530"/>
+    </row>
+    <row r="4531" spans="1:4">
+      <c r="A4531"/>
+    </row>
+    <row r="4532" spans="1:4">
+      <c r="A4532"/>
+    </row>
+    <row r="4533" spans="1:4">
+      <c r="A4533"/>
+    </row>
+    <row r="4534" spans="1:4">
+      <c r="A4534"/>
+    </row>
+    <row r="4535" spans="1:4">
+      <c r="A4535"/>
+    </row>
+    <row r="4536" spans="1:4">
+      <c r="A4536"/>
+    </row>
+    <row r="4537" spans="1:4">
+      <c r="A4537"/>
+    </row>
+    <row r="4538" spans="1:4">
+      <c r="A4538"/>
+    </row>
+    <row r="4539" spans="1:4">
+      <c r="A4539"/>
+    </row>
+    <row r="4540" spans="1:4">
+      <c r="A4540"/>
+    </row>
+    <row r="4541" spans="1:4">
+      <c r="A4541"/>
+    </row>
+    <row r="4542" spans="1:4">
+      <c r="A4542"/>
+    </row>
+    <row r="4543" spans="1:4">
+      <c r="A4543"/>
+    </row>
+    <row r="4544" spans="1:4">
+      <c r="A4544"/>
+    </row>
+    <row r="4545" spans="1:4">
+      <c r="A4545"/>
+    </row>
+    <row r="4546" spans="1:4">
+      <c r="A4546"/>
+    </row>
+    <row r="4547" spans="1:4">
+      <c r="A4547"/>
+    </row>
+    <row r="4548" spans="1:4">
+      <c r="A4548"/>
+    </row>
+    <row r="4549" spans="1:4">
+      <c r="A4549"/>
+    </row>
+    <row r="4550" spans="1:4">
+      <c r="A4550"/>
+    </row>
+    <row r="4551" spans="1:4">
+      <c r="A4551"/>
+    </row>
+    <row r="4552" spans="1:4">
+      <c r="A4552"/>
+    </row>
+    <row r="4553" spans="1:4">
+      <c r="A4553"/>
+    </row>
+    <row r="4554" spans="1:4">
+      <c r="A4554"/>
+    </row>
+    <row r="4555" spans="1:4">
+      <c r="A4555"/>
+    </row>
+    <row r="4556" spans="1:4">
+      <c r="A4556"/>
+    </row>
+    <row r="4557" spans="1:4">
+      <c r="A4557"/>
+    </row>
+    <row r="4558" spans="1:4">
+      <c r="A4558"/>
+    </row>
+    <row r="4559" spans="1:4">
+      <c r="A4559"/>
+    </row>
+    <row r="4560" spans="1:4">
+      <c r="A4560"/>
+    </row>
+    <row r="4561" spans="1:4">
+      <c r="A4561"/>
+    </row>
+    <row r="4562" spans="1:4">
+      <c r="A4562"/>
+    </row>
+    <row r="4563" spans="1:4">
+      <c r="A4563"/>
+    </row>
+    <row r="4564" spans="1:4">
+      <c r="A4564"/>
+    </row>
+    <row r="4565" spans="1:4">
+      <c r="A4565"/>
+    </row>
+    <row r="4566" spans="1:4">
+      <c r="A4566"/>
+    </row>
+    <row r="4567" spans="1:4">
+      <c r="A4567"/>
+    </row>
+    <row r="4568" spans="1:4">
+      <c r="A4568"/>
+    </row>
+    <row r="4569" spans="1:4">
+      <c r="A4569"/>
+    </row>
+    <row r="4570" spans="1:4">
+      <c r="A4570"/>
+    </row>
+    <row r="4571" spans="1:4">
+      <c r="A4571"/>
+    </row>
+    <row r="4572" spans="1:4">
+      <c r="A4572"/>
+    </row>
+    <row r="4573" spans="1:4">
+      <c r="A4573"/>
+    </row>
+    <row r="4574" spans="1:4">
+      <c r="A4574"/>
+    </row>
+    <row r="4575" spans="1:4">
+      <c r="A4575"/>
+    </row>
+    <row r="4576" spans="1:4">
+      <c r="A4576"/>
+    </row>
+    <row r="4577" spans="1:4">
+      <c r="A4577"/>
+    </row>
+    <row r="4578" spans="1:4">
+      <c r="A4578"/>
+    </row>
+    <row r="4579" spans="1:4">
+      <c r="A4579"/>
+    </row>
+    <row r="4580" spans="1:4">
+      <c r="A4580"/>
+    </row>
+    <row r="4581" spans="1:4">
+      <c r="A4581"/>
+    </row>
+    <row r="4582" spans="1:4">
+      <c r="A4582"/>
+    </row>
+    <row r="4583" spans="1:4">
+      <c r="A4583"/>
+    </row>
+    <row r="4584" spans="1:4">
+      <c r="A4584"/>
+    </row>
+    <row r="4585" spans="1:4">
+      <c r="A4585"/>
+    </row>
+    <row r="4586" spans="1:4">
+      <c r="A4586"/>
+    </row>
+    <row r="4587" spans="1:4">
+      <c r="A4587"/>
+    </row>
+    <row r="4588" spans="1:4">
+      <c r="A4588"/>
+    </row>
+    <row r="4589" spans="1:4">
+      <c r="A4589"/>
+    </row>
+    <row r="4590" spans="1:4">
+      <c r="A4590"/>
+    </row>
+    <row r="4591" spans="1:4">
+      <c r="A4591"/>
+    </row>
+    <row r="4592" spans="1:4">
+      <c r="A4592"/>
+    </row>
+    <row r="4593" spans="1:4">
+      <c r="A4593"/>
+    </row>
+    <row r="4594" spans="1:4">
+      <c r="A4594"/>
+    </row>
+    <row r="4595" spans="1:4">
+      <c r="A4595"/>
+    </row>
+    <row r="4596" spans="1:4">
+      <c r="A4596"/>
+    </row>
+    <row r="4597" spans="1:4">
+      <c r="A4597"/>
+    </row>
+    <row r="4598" spans="1:4">
+      <c r="A4598"/>
+    </row>
+    <row r="4599" spans="1:4">
+      <c r="A4599"/>
+    </row>
+    <row r="4600" spans="1:4">
+      <c r="A4600"/>
+    </row>
+    <row r="4601" spans="1:4">
+      <c r="A4601"/>
+    </row>
+    <row r="4602" spans="1:4">
+      <c r="A4602"/>
+    </row>
+    <row r="4603" spans="1:4">
+      <c r="A4603"/>
+    </row>
+    <row r="4604" spans="1:4">
+      <c r="A4604"/>
+    </row>
+    <row r="4605" spans="1:4">
+      <c r="A4605"/>
+    </row>
+    <row r="4606" spans="1:4">
+      <c r="A4606"/>
+    </row>
+    <row r="4607" spans="1:4">
+      <c r="A4607"/>
+    </row>
+    <row r="4608" spans="1:4">
+      <c r="A4608"/>
+    </row>
+    <row r="4609" spans="1:4">
+      <c r="A4609"/>
+    </row>
+    <row r="4610" spans="1:4">
+      <c r="A4610"/>
+    </row>
+    <row r="4611" spans="1:4">
+      <c r="A4611"/>
+    </row>
+    <row r="4612" spans="1:4">
+      <c r="A4612"/>
+    </row>
+    <row r="4613" spans="1:4">
+      <c r="A4613"/>
+    </row>
+    <row r="4614" spans="1:4">
+      <c r="A4614"/>
+    </row>
+    <row r="4615" spans="1:4">
+      <c r="A4615"/>
+    </row>
+    <row r="4616" spans="1:4">
+      <c r="A4616"/>
+    </row>
+    <row r="4617" spans="1:4">
+      <c r="A4617"/>
+    </row>
+    <row r="4618" spans="1:4">
+      <c r="A4618"/>
+    </row>
+    <row r="4619" spans="1:4">
+      <c r="A4619"/>
+    </row>
+    <row r="4620" spans="1:4">
+      <c r="A4620"/>
+    </row>
+    <row r="4621" spans="1:4">
+      <c r="A4621"/>
+    </row>
+    <row r="4622" spans="1:4">
+      <c r="A4622"/>
+    </row>
+    <row r="4623" spans="1:4">
+      <c r="A4623"/>
+    </row>
+    <row r="4624" spans="1:4">
+      <c r="A4624"/>
+    </row>
+    <row r="4625" spans="1:4">
+      <c r="A4625"/>
+    </row>
+    <row r="4626" spans="1:4">
+      <c r="A4626"/>
+    </row>
+    <row r="4627" spans="1:4">
+      <c r="A4627"/>
+    </row>
+    <row r="4628" spans="1:4">
+      <c r="A4628"/>
+    </row>
+    <row r="4629" spans="1:4">
+      <c r="A4629"/>
+    </row>
+    <row r="4630" spans="1:4">
+      <c r="A4630"/>
+    </row>
+    <row r="4631" spans="1:4">
+      <c r="A4631"/>
+    </row>
+    <row r="4632" spans="1:4">
+      <c r="A4632"/>
+    </row>
+    <row r="4633" spans="1:4">
+      <c r="A4633"/>
+    </row>
+    <row r="4634" spans="1:4">
+      <c r="A4634"/>
+    </row>
+    <row r="4635" spans="1:4">
+      <c r="A4635"/>
+    </row>
+    <row r="4636" spans="1:4">
+      <c r="A4636"/>
+    </row>
+    <row r="4637" spans="1:4">
+      <c r="A4637"/>
+    </row>
+    <row r="4638" spans="1:4">
+      <c r="A4638"/>
+    </row>
+    <row r="4639" spans="1:4">
+      <c r="A4639"/>
+    </row>
+    <row r="4640" spans="1:4">
+      <c r="A4640"/>
+    </row>
+    <row r="4641" spans="1:4">
+      <c r="A4641"/>
+    </row>
+    <row r="4642" spans="1:4">
+      <c r="A4642"/>
+    </row>
+    <row r="4643" spans="1:4">
+      <c r="A4643"/>
+    </row>
+    <row r="4644" spans="1:4">
+      <c r="A4644"/>
+    </row>
+    <row r="4645" spans="1:4">
+      <c r="A4645"/>
+    </row>
+    <row r="4646" spans="1:4">
+      <c r="A4646"/>
+    </row>
+    <row r="4647" spans="1:4">
+      <c r="A4647"/>
+    </row>
+    <row r="4648" spans="1:4">
+      <c r="A4648"/>
+    </row>
+    <row r="4649" spans="1:4">
+      <c r="A4649"/>
+    </row>
+    <row r="4650" spans="1:4">
+      <c r="A4650"/>
+    </row>
+    <row r="4651" spans="1:4">
+      <c r="A4651"/>
+    </row>
+    <row r="4652" spans="1:4">
+      <c r="A4652"/>
+    </row>
+    <row r="4653" spans="1:4">
+      <c r="A4653"/>
+    </row>
+    <row r="4654" spans="1:4">
+      <c r="A4654"/>
+    </row>
+    <row r="4655" spans="1:4">
+      <c r="A4655"/>
+    </row>
+    <row r="4656" spans="1:4">
+      <c r="A4656"/>
+    </row>
+    <row r="4657" spans="1:4">
+      <c r="A4657"/>
+    </row>
+    <row r="4658" spans="1:4">
+      <c r="A4658"/>
+    </row>
+    <row r="4659" spans="1:4">
+      <c r="A4659"/>
+    </row>
+    <row r="4660" spans="1:4">
+      <c r="A4660"/>
+    </row>
+    <row r="4661" spans="1:4">
+      <c r="A4661"/>
+    </row>
+    <row r="4662" spans="1:4">
+      <c r="A4662"/>
+    </row>
+    <row r="4663" spans="1:4">
+      <c r="A4663"/>
+    </row>
+    <row r="4664" spans="1:4">
+      <c r="A4664"/>
+    </row>
+    <row r="4665" spans="1:4">
+      <c r="A4665"/>
+    </row>
+    <row r="4666" spans="1:4">
+      <c r="A4666"/>
+    </row>
+    <row r="4667" spans="1:4">
+      <c r="A4667"/>
+    </row>
+    <row r="4668" spans="1:4">
+      <c r="A4668"/>
+    </row>
+    <row r="4669" spans="1:4">
+      <c r="A4669"/>
+    </row>
+    <row r="4670" spans="1:4">
+      <c r="A4670"/>
+    </row>
+    <row r="4671" spans="1:4">
+      <c r="A4671"/>
+    </row>
+    <row r="4672" spans="1:4">
+      <c r="A4672"/>
+    </row>
+    <row r="4673" spans="1:4">
+      <c r="A4673"/>
+    </row>
+    <row r="4674" spans="1:4">
+      <c r="A4674"/>
+    </row>
+    <row r="4675" spans="1:4">
+      <c r="A4675"/>
+    </row>
+    <row r="4676" spans="1:4">
+      <c r="A4676"/>
+    </row>
+    <row r="4677" spans="1:4">
+      <c r="A4677"/>
+    </row>
+    <row r="4678" spans="1:4">
+      <c r="A4678"/>
+    </row>
+    <row r="4679" spans="1:4">
+      <c r="A4679"/>
+    </row>
+    <row r="4680" spans="1:4">
+      <c r="A4680"/>
+    </row>
+    <row r="4681" spans="1:4">
+      <c r="A4681"/>
+    </row>
+    <row r="4682" spans="1:4">
+      <c r="A4682"/>
+    </row>
+    <row r="4683" spans="1:4">
+      <c r="A4683"/>
+    </row>
+    <row r="4684" spans="1:4">
+      <c r="A4684"/>
+    </row>
+    <row r="4685" spans="1:4">
+      <c r="A4685"/>
+    </row>
+    <row r="4686" spans="1:4">
+      <c r="A4686"/>
+    </row>
+    <row r="4687" spans="1:4">
+      <c r="A4687"/>
+    </row>
+    <row r="4688" spans="1:4">
+      <c r="A4688"/>
+    </row>
+    <row r="4689" spans="1:4">
+      <c r="A4689"/>
+    </row>
+    <row r="4690" spans="1:4">
+      <c r="A4690"/>
+    </row>
+    <row r="4691" spans="1:4">
+      <c r="A4691"/>
+    </row>
+    <row r="4692" spans="1:4">
+      <c r="A4692"/>
+    </row>
+    <row r="4693" spans="1:4">
+      <c r="A4693"/>
+    </row>
+    <row r="4694" spans="1:4">
+      <c r="A4694"/>
+    </row>
+    <row r="4695" spans="1:4">
+      <c r="A4695"/>
+    </row>
+    <row r="4696" spans="1:4">
+      <c r="A4696"/>
+    </row>
+    <row r="4697" spans="1:4">
+      <c r="A4697"/>
+    </row>
+    <row r="4698" spans="1:4">
+      <c r="A4698"/>
+    </row>
+    <row r="4699" spans="1:4">
+      <c r="A4699"/>
+    </row>
+    <row r="4700" spans="1:4">
+      <c r="A4700"/>
+    </row>
+    <row r="4701" spans="1:4">
+      <c r="A4701"/>
+    </row>
+    <row r="4702" spans="1:4">
+      <c r="A4702"/>
+    </row>
+    <row r="4703" spans="1:4">
+      <c r="A4703"/>
+    </row>
+    <row r="4704" spans="1:4">
+      <c r="A4704"/>
+    </row>
+    <row r="4705" spans="1:4">
+      <c r="A4705"/>
+    </row>
+    <row r="4706" spans="1:4">
+      <c r="A4706"/>
+    </row>
+    <row r="4707" spans="1:4">
+      <c r="A4707"/>
+    </row>
+    <row r="4708" spans="1:4">
+      <c r="A4708"/>
+    </row>
+    <row r="4709" spans="1:4">
+      <c r="A4709"/>
+    </row>
+    <row r="4710" spans="1:4">
+      <c r="A4710"/>
+    </row>
+    <row r="4711" spans="1:4">
+      <c r="A4711"/>
+    </row>
+    <row r="4712" spans="1:4">
+      <c r="A4712"/>
+    </row>
+    <row r="4713" spans="1:4">
+      <c r="A4713"/>
+    </row>
+    <row r="4714" spans="1:4">
+      <c r="A4714"/>
+    </row>
+    <row r="4715" spans="1:4">
+      <c r="A4715"/>
+    </row>
+    <row r="4716" spans="1:4">
+      <c r="A4716"/>
+    </row>
+    <row r="4717" spans="1:4">
+      <c r="A4717"/>
+    </row>
+    <row r="4718" spans="1:4">
+      <c r="A4718"/>
+    </row>
+    <row r="4719" spans="1:4">
+      <c r="A4719"/>
+    </row>
+    <row r="4720" spans="1:4">
+      <c r="A4720"/>
+    </row>
+    <row r="4721" spans="1:4">
+      <c r="A4721"/>
+    </row>
+    <row r="4722" spans="1:4">
+      <c r="A4722"/>
+    </row>
+    <row r="4723" spans="1:4">
+      <c r="A4723"/>
+    </row>
+    <row r="4724" spans="1:4">
+      <c r="A4724"/>
+    </row>
+    <row r="4725" spans="1:4">
+      <c r="A4725"/>
+    </row>
+    <row r="4726" spans="1:4">
+      <c r="A4726"/>
+    </row>
+    <row r="4727" spans="1:4">
+      <c r="A4727"/>
+    </row>
+    <row r="4728" spans="1:4">
+      <c r="A4728"/>
+    </row>
+    <row r="4729" spans="1:4">
+      <c r="A4729"/>
+    </row>
+    <row r="4730" spans="1:4">
+      <c r="A4730"/>
+    </row>
+    <row r="4731" spans="1:4">
+      <c r="A4731"/>
+    </row>
+    <row r="4732" spans="1:4">
+      <c r="A4732"/>
+    </row>
+    <row r="4733" spans="1:4">
+      <c r="A4733"/>
+    </row>
+    <row r="4734" spans="1:4">
+      <c r="A4734"/>
+    </row>
+    <row r="4735" spans="1:4">
+      <c r="A4735"/>
+    </row>
+    <row r="4736" spans="1:4">
+      <c r="A4736"/>
+    </row>
+    <row r="4737" spans="1:4">
+      <c r="A4737"/>
+    </row>
+    <row r="4738" spans="1:4">
+      <c r="A4738"/>
+    </row>
+    <row r="4739" spans="1:4">
+      <c r="A4739"/>
+    </row>
+    <row r="4740" spans="1:4">
+      <c r="A4740"/>
+    </row>
+    <row r="4741" spans="1:4">
+      <c r="A4741"/>
+    </row>
+    <row r="4742" spans="1:4">
+      <c r="A4742"/>
+    </row>
+    <row r="4743" spans="1:4">
+      <c r="A4743"/>
+    </row>
+    <row r="4744" spans="1:4">
+      <c r="A4744"/>
+    </row>
+    <row r="4745" spans="1:4">
+      <c r="A4745"/>
+    </row>
+    <row r="4746" spans="1:4">
+      <c r="A4746"/>
+    </row>
+    <row r="4747" spans="1:4">
+      <c r="A4747"/>
+    </row>
+    <row r="4748" spans="1:4">
+      <c r="A4748"/>
+    </row>
+    <row r="4749" spans="1:4">
+      <c r="A4749"/>
+    </row>
+    <row r="4750" spans="1:4">
+      <c r="A4750"/>
+    </row>
+    <row r="4751" spans="1:4">
+      <c r="A4751"/>
+    </row>
+    <row r="4752" spans="1:4">
+      <c r="A4752"/>
+    </row>
+    <row r="4753" spans="1:4">
+      <c r="A4753"/>
+    </row>
+    <row r="4754" spans="1:4">
+      <c r="A4754"/>
+    </row>
+    <row r="4755" spans="1:4">
+      <c r="A4755"/>
+    </row>
+    <row r="4756" spans="1:4">
+      <c r="A4756"/>
+    </row>
+    <row r="4757" spans="1:4">
+      <c r="A4757"/>
+    </row>
+    <row r="4758" spans="1:4">
+      <c r="A4758"/>
+    </row>
+    <row r="4759" spans="1:4">
+      <c r="A4759"/>
+    </row>
+    <row r="4760" spans="1:4">
+      <c r="A4760"/>
+    </row>
+    <row r="4761" spans="1:4">
+      <c r="A4761"/>
+    </row>
+    <row r="4762" spans="1:4">
+      <c r="A4762"/>
+    </row>
+    <row r="4763" spans="1:4">
+      <c r="A4763"/>
+    </row>
+    <row r="4764" spans="1:4">
+      <c r="A4764"/>
+    </row>
+    <row r="4765" spans="1:4">
+      <c r="A4765"/>
+    </row>
+    <row r="4766" spans="1:4">
+      <c r="A4766"/>
+    </row>
+    <row r="4767" spans="1:4">
+      <c r="A4767"/>
+    </row>
+    <row r="4768" spans="1:4">
+      <c r="A4768"/>
+    </row>
+    <row r="4769" spans="1:4">
+      <c r="A4769"/>
+    </row>
+    <row r="4770" spans="1:4">
+      <c r="A4770"/>
+    </row>
+    <row r="4771" spans="1:4">
+      <c r="A4771"/>
+    </row>
+    <row r="4772" spans="1:4">
+      <c r="A4772"/>
+    </row>
+    <row r="4773" spans="1:4">
+      <c r="A4773"/>
+    </row>
+    <row r="4774" spans="1:4">
+      <c r="A4774"/>
+    </row>
+    <row r="4775" spans="1:4">
+      <c r="A4775"/>
+    </row>
+    <row r="4776" spans="1:4">
+      <c r="A4776"/>
+    </row>
+    <row r="4777" spans="1:4">
+      <c r="A4777"/>
+    </row>
+    <row r="4778" spans="1:4">
+      <c r="A4778"/>
+    </row>
+    <row r="4779" spans="1:4">
+      <c r="A4779"/>
+    </row>
+    <row r="4780" spans="1:4">
+      <c r="A4780"/>
+    </row>
+    <row r="4781" spans="1:4">
+      <c r="A4781"/>
+    </row>
+    <row r="4782" spans="1:4">
+      <c r="A4782"/>
+    </row>
+    <row r="4783" spans="1:4">
+      <c r="A4783"/>
+    </row>
+    <row r="4784" spans="1:4">
+      <c r="A4784"/>
+    </row>
+    <row r="4785" spans="1:4">
+      <c r="A4785"/>
+    </row>
+    <row r="4786" spans="1:4">
+      <c r="A4786"/>
+    </row>
+    <row r="4787" spans="1:4">
+      <c r="A4787"/>
+    </row>
+    <row r="4788" spans="1:4">
+      <c r="A4788"/>
+    </row>
+    <row r="4789" spans="1:4">
+      <c r="A4789"/>
+    </row>
+    <row r="4790" spans="1:4">
+      <c r="A4790"/>
+    </row>
+    <row r="4791" spans="1:4">
+      <c r="A4791"/>
+    </row>
+    <row r="4792" spans="1:4">
+      <c r="A4792"/>
+    </row>
+    <row r="4793" spans="1:4">
+      <c r="A4793"/>
+    </row>
+    <row r="4794" spans="1:4">
+      <c r="A4794"/>
+    </row>
+    <row r="4795" spans="1:4">
+      <c r="A4795"/>
+    </row>
+    <row r="4796" spans="1:4">
+      <c r="A4796"/>
+    </row>
+    <row r="4797" spans="1:4">
+      <c r="A4797"/>
+    </row>
+    <row r="4798" spans="1:4">
+      <c r="A4798"/>
+    </row>
+    <row r="4799" spans="1:4">
+      <c r="A4799"/>
+    </row>
+    <row r="4800" spans="1:4">
+      <c r="A4800"/>
+    </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <printOptions gridLines="false" gridLinesSet="true"/>

</xml_diff>